<commit_message>
Updated code on timestamp:   18-05-2021 - 21:48:40.29
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="502">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1705,6 +1705,9 @@
   </si>
   <si>
     <t>CP/Leet_coinchange.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists - LeetCode</t>
   </si>
 </sst>
 </file>
@@ -3499,7 +3502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -6896,8 +6899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7256,6 +7259,9 @@
       <c r="G19" s="5">
         <v>0</v>
       </c>
+      <c r="H19" s="16" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
@@ -7384,6 +7390,7 @@
     <hyperlink ref="K10" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
     <hyperlink ref="K11" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
     <hyperlink ref="K12" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
+    <hyperlink ref="H19" r:id="rId10" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   19-05-2021 -  2:27:39.55
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="526">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1733,12 +1733,60 @@
   <si>
     <t>Palindrome Linked List - LeetCode</t>
   </si>
+  <si>
+    <t>LEETCODE</t>
+  </si>
+  <si>
+    <t>Linked List Cycle - LeetCode</t>
+  </si>
+  <si>
+    <t>Valid Parentheses - LeetCode</t>
+  </si>
+  <si>
+    <t>Linked List Cycle II - LeetCode</t>
+  </si>
+  <si>
+    <t>Add Two Numbers - LeetCode</t>
+  </si>
+  <si>
+    <t>premium</t>
+  </si>
+  <si>
+    <t>(306) Mathmatical Proof of Detection of Cycle in A LinkedList | In Hindi - YouTube</t>
+  </si>
+  <si>
+    <t>CP/OddEvenLinklist.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/RemoveDuplicatesFromSortedLL.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/Linklist_To_Stack_Adapter.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/LinklistToQueueAdapter.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/KthNodeFromEndOfLiklist.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/MidOfLinklist.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/ReverseLinklist_Iterative.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/ReverseLinklist_Pointer.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/KReverseinLL.java at main · spartan4cs/CP (github.com)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1814,6 +1862,13 @@
       <color rgb="FF2A2E2E"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="16">
@@ -2053,7 +2108,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2321,11 +2376,19 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="10" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="8" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -3668,7 +3731,7 @@
       <c r="F9" s="25" t="s">
         <v>497</v>
       </c>
-      <c r="G9" s="96" t="s">
+      <c r="G9" s="95" t="s">
         <v>499</v>
       </c>
       <c r="H9" s="10"/>
@@ -5252,10 +5315,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6099,6 +6162,11 @@
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
         <v>421</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="16" t="s">
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -6139,9 +6207,10 @@
     <hyperlink ref="I18" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java"/>
     <hyperlink ref="I19" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java"/>
     <hyperlink ref="I20" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java"/>
+    <hyperlink ref="B49" r:id="rId37" display="https://leetcode.com/problems/valid-parentheses/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId38"/>
 </worksheet>
 </file>
 
@@ -6173,15 +6242,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="76" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="100" t="s">
         <v>350</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
       <c r="I2" s="77"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6921,16 +6990,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="29"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="51.85546875" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="39.7109375" customWidth="1"/>
@@ -7169,6 +7239,9 @@
       <c r="I13" s="16" t="s">
         <v>508</v>
       </c>
+      <c r="K13" s="16" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
@@ -7189,6 +7262,9 @@
       <c r="H14" s="18" t="s">
         <v>471</v>
       </c>
+      <c r="K14" s="16" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
@@ -7209,6 +7285,9 @@
       <c r="H15" s="18" t="s">
         <v>469</v>
       </c>
+      <c r="K15" s="16" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
@@ -7229,8 +7308,11 @@
       <c r="H16" s="18" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="K16" s="16" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>13</v>
       </c>
@@ -7248,6 +7330,9 @@
       </c>
       <c r="H17" s="18" t="s">
         <v>473</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -7269,6 +7354,9 @@
       <c r="H18" s="18" t="s">
         <v>472</v>
       </c>
+      <c r="K18" s="16" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
@@ -7329,6 +7417,9 @@
       <c r="H21" s="16" t="s">
         <v>505</v>
       </c>
+      <c r="K21" s="16" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
@@ -7340,6 +7431,9 @@
       <c r="E22" t="s">
         <v>33</v>
       </c>
+      <c r="K22" s="16" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
@@ -7351,6 +7445,9 @@
       <c r="E23" t="s">
         <v>33</v>
       </c>
+      <c r="K23" s="16" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
@@ -7418,18 +7515,99 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="16" t="s">
+    <row r="30" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:11" s="97" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A32" s="96"/>
+      <c r="D32" s="98" t="s">
+        <v>510</v>
+      </c>
+      <c r="G32" s="99"/>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D34" s="16" t="s">
+        <v>508</v>
+      </c>
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D35" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="F35" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D36" s="16" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="16" t="s">
+      <c r="F36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D37" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="F37" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D38" s="16" t="s">
+        <v>513</v>
+      </c>
+      <c r="F38" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="K38" s="16"/>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D39" s="16" t="s">
+        <v>505</v>
+      </c>
+      <c r="F39" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D40" s="16" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D41" s="16" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="16" t="s">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C42" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="D42" s="16" t="s">
         <v>507</v>
       </c>
     </row>
@@ -7448,10 +7626,26 @@
     <hyperlink ref="K19" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Leet_mergeTwoSorterLinklist.java"/>
     <hyperlink ref="K20" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistMergeSort.java"/>
     <hyperlink ref="H21" r:id="rId13" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
-    <hyperlink ref="D34" r:id="rId14" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/"/>
-    <hyperlink ref="D35" r:id="rId15" display="https://leetcode.com/problems/remove-duplicates-from-an-unsorted-linked-list/"/>
-    <hyperlink ref="I13" r:id="rId16" display="https://leetcode.com/problems/reverse-linked-list/"/>
-    <hyperlink ref="D33" r:id="rId17" display="https://leetcode.com/problems/palindrome-linked-list/"/>
+    <hyperlink ref="D42" r:id="rId14" display="https://leetcode.com/problems/remove-duplicates-from-an-unsorted-linked-list/"/>
+    <hyperlink ref="I13" r:id="rId15" display="https://leetcode.com/problems/reverse-linked-list/"/>
+    <hyperlink ref="D39" r:id="rId16" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
+    <hyperlink ref="D35" r:id="rId17" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
+    <hyperlink ref="D34" r:id="rId18" display="https://leetcode.com/problems/reverse-linked-list/"/>
+    <hyperlink ref="D37" r:id="rId19" display="https://leetcode.com/problems/linked-list-cycle/"/>
+    <hyperlink ref="D38" r:id="rId20" display="https://leetcode.com/problems/linked-list-cycle-ii/"/>
+    <hyperlink ref="D41" r:id="rId21" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/"/>
+    <hyperlink ref="D36" r:id="rId22" display="https://leetcode.com/problems/palindrome-linked-list/"/>
+    <hyperlink ref="D40" r:id="rId23" display="https://leetcode.com/problems/add-two-numbers/"/>
+    <hyperlink ref="H38" r:id="rId24" display="https://www.youtube.com/watch?v=dpqpgnTHiLs"/>
+    <hyperlink ref="K22" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/OddEvenLinklist.java"/>
+    <hyperlink ref="K21" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/RemoveDuplicatesFromSortedLL.java"/>
+    <hyperlink ref="K15" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java"/>
+    <hyperlink ref="K16" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistToQueueAdapter.java"/>
+    <hyperlink ref="K17" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KthNodeFromEndOfLiklist.java"/>
+    <hyperlink ref="K18" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/MidOfLinklist.java"/>
+    <hyperlink ref="K13" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Iterative.java"/>
+    <hyperlink ref="K14" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Pointer.java"/>
+    <hyperlink ref="K23" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KReverseinLL.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   20-05-2021 -  0:07:07.53
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="526">
   <si>
     <t>TOPIC</t>
   </si>
@@ -6992,8 +6992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7601,6 +7601,12 @@
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D41" s="16" t="s">
         <v>506</v>
+      </c>
+      <c r="F41" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code on timestamp:   20-05-2021 -  1:27:45.43
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="526">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1786,7 +1786,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1870,8 +1870,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1956,6 +1963,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -2092,7 +2104,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2107,8 +2119,9 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2390,8 +2403,14 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="14" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
     <cellStyle name="20% - Accent6" xfId="9" builtinId="50"/>
     <cellStyle name="40% - Accent1" xfId="11" builtinId="31"/>
@@ -2402,6 +2421,7 @@
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Accent5" xfId="13" builtinId="45"/>
+    <cellStyle name="Bad" xfId="14" builtinId="27"/>
     <cellStyle name="Good" xfId="8" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -6992,7 +7012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
@@ -7661,8 +7681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7722,87 +7742,147 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="101" t="s">
         <v>212</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="101" t="s">
         <v>213</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="101" t="s">
         <v>214</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="101" t="s">
         <v>215</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="101" t="s">
         <v>216</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="101" t="s">
         <v>217</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="37" t="s">
         <v>218</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="101" t="s">
         <v>219</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="101" t="s">
         <v>220</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="101" t="s">
         <v>221</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="86" t="s">
         <v>222</v>
       </c>
     </row>
@@ -7810,7 +7890,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="86" t="s">
         <v>223</v>
       </c>
     </row>
@@ -7818,7 +7898,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="86" t="s">
         <v>224</v>
       </c>
     </row>
@@ -7826,7 +7906,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="86" t="s">
         <v>225</v>
       </c>
     </row>
@@ -7834,7 +7914,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="86" t="s">
         <v>226</v>
       </c>
     </row>
@@ -7842,7 +7922,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="86" t="s">
         <v>227</v>
       </c>
     </row>
@@ -7850,7 +7930,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="86" t="s">
         <v>228</v>
       </c>
     </row>
@@ -7858,7 +7938,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="86" t="s">
         <v>229</v>
       </c>
     </row>
@@ -7866,7 +7946,7 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="86" t="s">
         <v>230</v>
       </c>
     </row>
@@ -7874,7 +7954,7 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="86" t="s">
         <v>231</v>
       </c>
     </row>
@@ -7882,7 +7962,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="102" t="s">
         <v>232</v>
       </c>
     </row>
@@ -7890,7 +7970,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="102" t="s">
         <v>233</v>
       </c>
     </row>
@@ -7898,7 +7978,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="102" t="s">
         <v>234</v>
       </c>
     </row>
@@ -7906,7 +7986,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="102" t="s">
         <v>235</v>
       </c>
     </row>
@@ -7914,7 +7994,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="102" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7922,7 +8002,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="102" t="s">
         <v>237</v>
       </c>
     </row>
@@ -7930,7 +8010,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="102" t="s">
         <v>238</v>
       </c>
     </row>
@@ -7938,7 +8018,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="102" t="s">
         <v>239</v>
       </c>
     </row>
@@ -7946,7 +8026,7 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="D32" s="25" t="s">
+      <c r="D32" s="102" t="s">
         <v>240</v>
       </c>
     </row>
@@ -7954,7 +8034,7 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="102" t="s">
         <v>241</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   20-05-2021 -  2:30:21.23
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -2121,7 +2121,7 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2233,9 +2233,6 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2380,9 +2377,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="12" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2400,14 +2394,23 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="14" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="8" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="14" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -2853,7 +2856,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D14" sqref="D14:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2913,7 +2916,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="96" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2921,7 +2924,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="96" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2929,7 +2932,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="96" t="s">
         <v>267</v>
       </c>
     </row>
@@ -2937,7 +2940,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="96" t="s">
         <v>268</v>
       </c>
     </row>
@@ -2945,7 +2948,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="96" t="s">
         <v>269</v>
       </c>
     </row>
@@ -2953,7 +2956,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="96" t="s">
         <v>270</v>
       </c>
     </row>
@@ -2961,7 +2964,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="96" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2969,7 +2972,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="96" t="s">
         <v>272</v>
       </c>
     </row>
@@ -2977,7 +2980,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="96" t="s">
         <v>273</v>
       </c>
     </row>
@@ -2985,7 +2988,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="96" t="s">
         <v>274</v>
       </c>
     </row>
@@ -2993,7 +2996,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="83" t="s">
         <v>275</v>
       </c>
     </row>
@@ -3001,7 +3004,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="83" t="s">
         <v>276</v>
       </c>
     </row>
@@ -3009,7 +3012,7 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="83" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3017,7 +3020,7 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="83" t="s">
         <v>278</v>
       </c>
     </row>
@@ -3025,7 +3028,7 @@
       <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="83" t="s">
         <v>279</v>
       </c>
     </row>
@@ -3033,7 +3036,7 @@
       <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="83" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3041,7 +3044,7 @@
       <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="83" t="s">
         <v>281</v>
       </c>
     </row>
@@ -3049,7 +3052,7 @@
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="83" t="s">
         <v>282</v>
       </c>
     </row>
@@ -3057,7 +3060,7 @@
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="83" t="s">
         <v>283</v>
       </c>
     </row>
@@ -3065,7 +3068,7 @@
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="83" t="s">
         <v>284</v>
       </c>
     </row>
@@ -3079,7 +3082,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D4" sqref="D4:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3137,7 +3140,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="98" t="s">
         <v>285</v>
       </c>
     </row>
@@ -3145,7 +3148,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="98" t="s">
         <v>286</v>
       </c>
     </row>
@@ -3153,7 +3156,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="98" t="s">
         <v>287</v>
       </c>
     </row>
@@ -3161,7 +3164,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="98" t="s">
         <v>288</v>
       </c>
     </row>
@@ -3169,7 +3172,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="98" t="s">
         <v>289</v>
       </c>
     </row>
@@ -3177,7 +3180,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="98" t="s">
         <v>290</v>
       </c>
     </row>
@@ -3185,7 +3188,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="98" t="s">
         <v>291</v>
       </c>
     </row>
@@ -3193,7 +3196,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="98" t="s">
         <v>292</v>
       </c>
     </row>
@@ -3201,7 +3204,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="98" t="s">
         <v>293</v>
       </c>
     </row>
@@ -3209,7 +3212,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="98" t="s">
         <v>294</v>
       </c>
     </row>
@@ -3223,7 +3226,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="D14" sqref="D14:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3281,7 +3284,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="96" t="s">
         <v>295</v>
       </c>
     </row>
@@ -3289,7 +3292,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="96" t="s">
         <v>296</v>
       </c>
     </row>
@@ -3297,7 +3300,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="96" t="s">
         <v>297</v>
       </c>
     </row>
@@ -3305,7 +3308,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="96" t="s">
         <v>298</v>
       </c>
     </row>
@@ -3313,7 +3316,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="96" t="s">
         <v>299</v>
       </c>
     </row>
@@ -3321,7 +3324,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="96" t="s">
         <v>300</v>
       </c>
     </row>
@@ -3329,7 +3332,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="96" t="s">
         <v>301</v>
       </c>
     </row>
@@ -3337,7 +3340,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="96" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3345,7 +3348,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="96" t="s">
         <v>303</v>
       </c>
     </row>
@@ -3353,7 +3356,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="96" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3361,7 +3364,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="83" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3369,7 +3372,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="83" t="s">
         <v>306</v>
       </c>
     </row>
@@ -3377,7 +3380,7 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="83" t="s">
         <v>307</v>
       </c>
     </row>
@@ -3385,7 +3388,7 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="83" t="s">
         <v>308</v>
       </c>
     </row>
@@ -3399,7 +3402,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D14" sqref="D14:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,7 +3463,7 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="96" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3468,7 +3471,7 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="96" t="s">
         <v>311</v>
       </c>
     </row>
@@ -3476,7 +3479,7 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="96" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3484,7 +3487,7 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="96" t="s">
         <v>313</v>
       </c>
     </row>
@@ -3492,7 +3495,7 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="96" t="s">
         <v>314</v>
       </c>
     </row>
@@ -3500,7 +3503,7 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="96" t="s">
         <v>315</v>
       </c>
     </row>
@@ -3508,7 +3511,7 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="96" t="s">
         <v>316</v>
       </c>
     </row>
@@ -3516,7 +3519,7 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="96" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3524,7 +3527,7 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="96" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3532,7 +3535,7 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="96" t="s">
         <v>319</v>
       </c>
     </row>
@@ -3540,7 +3543,7 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="83" t="s">
         <v>320</v>
       </c>
     </row>
@@ -3548,7 +3551,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="83" t="s">
         <v>321</v>
       </c>
     </row>
@@ -3556,7 +3559,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="83" t="s">
         <v>322</v>
       </c>
     </row>
@@ -3564,7 +3567,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="83" t="s">
         <v>323</v>
       </c>
     </row>
@@ -3572,7 +3575,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="83" t="s">
         <v>324</v>
       </c>
     </row>
@@ -3580,7 +3583,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="83" t="s">
         <v>325</v>
       </c>
     </row>
@@ -3588,7 +3591,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="83" t="s">
         <v>326</v>
       </c>
     </row>
@@ -3596,7 +3599,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="83" t="s">
         <v>310</v>
       </c>
     </row>
@@ -3716,7 +3719,7 @@
         <v>452</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="80" t="s">
         <v>474</v>
       </c>
       <c r="E8" s="5">
@@ -3751,7 +3754,7 @@
       <c r="F9" s="25" t="s">
         <v>497</v>
       </c>
-      <c r="G9" s="95" t="s">
+      <c r="G9" s="91" t="s">
         <v>499</v>
       </c>
       <c r="H9" s="10"/>
@@ -3918,7 +3921,7 @@
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="41" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -3947,7 +3950,7 @@
       <c r="B5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="42" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -3976,7 +3979,7 @@
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="42" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -4005,7 +4008,7 @@
       <c r="B7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="42" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -4034,7 +4037,7 @@
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="42" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -4060,7 +4063,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="42" t="s">
         <v>81</v>
       </c>
       <c r="G9" s="2">
@@ -4083,7 +4086,7 @@
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="42" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -4115,7 +4118,7 @@
       <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -4147,7 +4150,7 @@
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="44" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -4176,7 +4179,7 @@
       <c r="B13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="45" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -4208,7 +4211,7 @@
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="45" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -4240,7 +4243,7 @@
       <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="45" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -4266,7 +4269,7 @@
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="45" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -4292,7 +4295,7 @@
       <c r="B17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="46" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -4321,7 +4324,7 @@
       <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="47" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -4347,7 +4350,7 @@
       <c r="B19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="51" t="s">
+      <c r="D19" s="48" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -4370,7 +4373,7 @@
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="48" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -4393,7 +4396,7 @@
       <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="51" t="s">
+      <c r="D21" s="48" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -4416,7 +4419,7 @@
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="49" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -4439,7 +4442,7 @@
       <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="53" t="s">
+      <c r="D23" s="50" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -4468,7 +4471,7 @@
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="54" t="s">
+      <c r="D24" s="51" t="s">
         <v>20</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -4497,7 +4500,7 @@
       <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="51" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -4524,7 +4527,7 @@
       <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="D26" s="51" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -4551,7 +4554,7 @@
       <c r="B27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="54" t="s">
+      <c r="D27" s="51" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -4581,7 +4584,7 @@
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" s="51" t="s">
         <v>24</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -4608,7 +4611,7 @@
       <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="52" t="s">
         <v>25</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -4638,7 +4641,7 @@
       <c r="B30" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="59" t="s">
+      <c r="D30" s="56" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -4668,7 +4671,7 @@
       <c r="B31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="56" t="s">
+      <c r="D31" s="53" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -4698,7 +4701,7 @@
       <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="57" t="s">
+      <c r="D32" s="54" t="s">
         <v>133</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -4722,7 +4725,7 @@
       <c r="K32" s="16"/>
     </row>
     <row r="33" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="57" t="s">
+      <c r="D33" s="54" t="s">
         <v>134</v>
       </c>
       <c r="G33" s="2">
@@ -4740,7 +4743,7 @@
       <c r="B34" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="58" t="s">
+      <c r="D34" s="55" t="s">
         <v>28</v>
       </c>
       <c r="E34" s="5" t="s">
@@ -4772,7 +4775,7 @@
       <c r="K36" s="16"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D37" s="83"/>
+      <c r="D37" s="80"/>
       <c r="K37" s="16"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -4889,7 +4892,7 @@
       <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="83" t="s">
         <v>64</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -4915,7 +4918,7 @@
       <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="83" t="s">
         <v>66</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -4941,7 +4944,7 @@
       <c r="A8" s="13">
         <v>3</v>
       </c>
-      <c r="D8" s="86" t="s">
+      <c r="D8" s="83" t="s">
         <v>65</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -4961,7 +4964,7 @@
       <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="D9" s="87" t="s">
+      <c r="D9" s="84" t="s">
         <v>140</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -4984,7 +4987,7 @@
       <c r="A10" s="13">
         <v>5</v>
       </c>
-      <c r="D10" s="87" t="s">
+      <c r="D10" s="84" t="s">
         <v>140</v>
       </c>
       <c r="F10" s="23" t="s">
@@ -5001,10 +5004,10 @@
       <c r="A11" s="13">
         <v>6</v>
       </c>
-      <c r="D11" s="87" t="s">
+      <c r="D11" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="F11" s="82" t="s">
+      <c r="F11" s="79" t="s">
         <v>34</v>
       </c>
       <c r="G11" s="5">
@@ -5021,7 +5024,7 @@
       <c r="A12" s="13">
         <v>7</v>
       </c>
-      <c r="D12" s="87" t="s">
+      <c r="D12" s="84" t="s">
         <v>141</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -5041,7 +5044,7 @@
       <c r="A13" s="13">
         <v>8</v>
       </c>
-      <c r="D13" s="87" t="s">
+      <c r="D13" s="84" t="s">
         <v>145</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -5067,7 +5070,7 @@
       <c r="A14" s="13">
         <v>9</v>
       </c>
-      <c r="D14" s="85" t="s">
+      <c r="D14" s="82" t="s">
         <v>150</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -5093,10 +5096,10 @@
       <c r="A15" s="13">
         <v>10</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="81" t="s">
         <v>480</v>
       </c>
-      <c r="D15" s="85" t="s">
+      <c r="D15" s="82" t="s">
         <v>152</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -5122,7 +5125,7 @@
       <c r="A16" s="13">
         <v>11</v>
       </c>
-      <c r="D16" s="85" t="s">
+      <c r="D16" s="82" t="s">
         <v>154</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -5145,7 +5148,7 @@
       <c r="A17" s="13">
         <v>12</v>
       </c>
-      <c r="D17" s="87" t="s">
+      <c r="D17" s="84" t="s">
         <v>155</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -5168,7 +5171,7 @@
       <c r="A18" s="13">
         <v>13</v>
       </c>
-      <c r="D18" s="87" t="s">
+      <c r="D18" s="84" t="s">
         <v>158</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -5191,7 +5194,7 @@
       <c r="A19" s="13">
         <v>14</v>
       </c>
-      <c r="D19" s="87" t="s">
+      <c r="D19" s="84" t="s">
         <v>160</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -5214,7 +5217,7 @@
       <c r="A20" s="13">
         <v>15</v>
       </c>
-      <c r="D20" s="87" t="s">
+      <c r="D20" s="84" t="s">
         <v>163</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -5234,7 +5237,7 @@
       <c r="A21" s="13">
         <v>16</v>
       </c>
-      <c r="D21" s="87" t="s">
+      <c r="D21" s="84" t="s">
         <v>164</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -5254,7 +5257,7 @@
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="D22" s="87" t="s">
+      <c r="D22" s="84" t="s">
         <v>167</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -5274,7 +5277,7 @@
       <c r="A23" s="13">
         <v>18</v>
       </c>
-      <c r="D23" s="88" t="s">
+      <c r="D23" s="85" t="s">
         <v>175</v>
       </c>
       <c r="I23" s="15" t="s">
@@ -5285,12 +5288,12 @@
       <c r="A24" s="13">
         <v>19</v>
       </c>
-      <c r="D24" s="88" t="s">
+      <c r="D24" s="85" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="68"/>
+      <c r="D25" s="65"/>
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
@@ -5413,7 +5416,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -5439,7 +5442,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="58" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -5465,7 +5468,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="59" t="s">
         <v>337</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -5491,7 +5494,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="51" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -5517,7 +5520,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="51" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -5540,16 +5543,16 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="73" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="74">
+      <c r="C9" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="71">
         <v>5</v>
       </c>
       <c r="G9" s="10" t="s">
@@ -5563,7 +5566,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="62" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -5592,7 +5595,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="61" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -5618,7 +5621,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="61" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -5644,16 +5647,16 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="73" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="74">
+      <c r="C13" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="71">
         <v>3</v>
       </c>
       <c r="F13" s="10" t="s">
@@ -5670,7 +5673,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="64" t="s">
         <v>48</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -5696,7 +5699,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="64" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -5719,7 +5722,7 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="64" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -5742,7 +5745,7 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="51" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -5765,7 +5768,7 @@
       <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="51" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -5785,7 +5788,7 @@
       <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="51" t="s">
         <v>54</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -5814,16 +5817,16 @@
       <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="69" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="71">
+      <c r="C20" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="68">
         <v>3</v>
       </c>
       <c r="G20" s="10" t="s">
@@ -5943,7 +5946,7 @@
       <c r="G36" s="10" t="s">
         <v>378</v>
       </c>
-      <c r="H36" s="63"/>
+      <c r="H36" s="60"/>
       <c r="I36" s="31"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -5965,7 +5968,7 @@
       <c r="F37" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="H37" s="63"/>
+      <c r="H37" s="60"/>
       <c r="I37" s="31"/>
     </row>
     <row r="38" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6238,7 +6241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -6261,23 +6264,23 @@
       </c>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:9" s="76" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="100" t="s">
+    <row r="2" spans="1:9" s="73" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A2" s="99" t="s">
         <v>350</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="I2" s="77"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="76" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="28" t="s">
@@ -6286,7 +6289,7 @@
       <c r="D3" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="72" t="s">
         <v>491</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -6306,7 +6309,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="77" t="s">
         <v>414</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -6331,7 +6334,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="48" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="5"/>
@@ -6348,7 +6351,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="48" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -6371,7 +6374,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="48" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -6394,7 +6397,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="48" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -6417,7 +6420,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="48" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -6440,7 +6443,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="49" t="s">
         <v>61</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -6453,7 +6456,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="10"/>
-      <c r="G10" s="81" t="s">
+      <c r="G10" s="78" t="s">
         <v>447</v>
       </c>
       <c r="H10" s="11"/>
@@ -6475,7 +6478,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="78" t="s">
+      <c r="F11" s="75" t="s">
         <v>410</v>
       </c>
       <c r="G11" s="10" t="s">
@@ -6525,8 +6528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6585,7 +6588,7 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="86" t="s">
         <v>179</v>
       </c>
       <c r="E4" t="s">
@@ -6599,7 +6602,7 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="86" t="s">
         <v>180</v>
       </c>
       <c r="E5" t="s">
@@ -6613,7 +6616,7 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="89" t="s">
+      <c r="D6" s="86" t="s">
         <v>181</v>
       </c>
       <c r="E6" t="s">
@@ -6627,7 +6630,7 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="89" t="s">
+      <c r="D7" s="86" t="s">
         <v>182</v>
       </c>
       <c r="E7" t="s">
@@ -6641,7 +6644,7 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="89" t="s">
+      <c r="D8" s="86" t="s">
         <v>183</v>
       </c>
       <c r="E8" t="s">
@@ -6655,7 +6658,7 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="89" t="s">
+      <c r="D9" s="86" t="s">
         <v>184</v>
       </c>
       <c r="E9" t="s">
@@ -6669,7 +6672,7 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="90" t="s">
+      <c r="D10" s="87" t="s">
         <v>185</v>
       </c>
       <c r="E10" t="s">
@@ -6683,7 +6686,7 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="90" t="s">
+      <c r="D11" s="87" t="s">
         <v>186</v>
       </c>
       <c r="E11" t="s">
@@ -6697,7 +6700,7 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="90" t="s">
+      <c r="D12" s="87" t="s">
         <v>187</v>
       </c>
       <c r="E12" t="s">
@@ -6711,7 +6714,7 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="90" t="s">
+      <c r="D13" s="87" t="s">
         <v>188</v>
       </c>
       <c r="E13" t="s">
@@ -6725,7 +6728,7 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="90" t="s">
+      <c r="D14" s="87" t="s">
         <v>189</v>
       </c>
       <c r="E14" t="s">
@@ -6739,7 +6742,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="90" t="s">
+      <c r="D15" s="87" t="s">
         <v>190</v>
       </c>
       <c r="E15" t="s">
@@ -6753,7 +6756,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="92" t="s">
+      <c r="D16" s="103" t="s">
         <v>191</v>
       </c>
       <c r="E16" t="s">
@@ -6767,7 +6770,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="92" t="s">
+      <c r="D17" s="103" t="s">
         <v>192</v>
       </c>
       <c r="E17" t="s">
@@ -6781,7 +6784,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="92" t="s">
+      <c r="D18" s="103" t="s">
         <v>193</v>
       </c>
       <c r="E18" t="s">
@@ -6795,7 +6798,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="92" t="s">
+      <c r="D19" s="103" t="s">
         <v>194</v>
       </c>
       <c r="E19" t="s">
@@ -6809,7 +6812,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="93" t="s">
+      <c r="D20" s="89" t="s">
         <v>195</v>
       </c>
       <c r="E20" t="s">
@@ -6823,7 +6826,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="93" t="s">
+      <c r="D21" s="89" t="s">
         <v>196</v>
       </c>
       <c r="E21" t="s">
@@ -6837,7 +6840,7 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="D22" s="93" t="s">
+      <c r="D22" s="89" t="s">
         <v>197</v>
       </c>
       <c r="E22" t="s">
@@ -6851,7 +6854,7 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="D23" s="93" t="s">
+      <c r="D23" s="89" t="s">
         <v>198</v>
       </c>
       <c r="E23" t="s">
@@ -6865,7 +6868,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="D24" s="94" t="s">
+      <c r="D24" s="90" t="s">
         <v>199</v>
       </c>
       <c r="E24" t="s">
@@ -6879,7 +6882,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="D25" s="94" t="s">
+      <c r="D25" s="90" t="s">
         <v>200</v>
       </c>
       <c r="E25" t="s">
@@ -6893,7 +6896,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="D26" s="94" t="s">
+      <c r="D26" s="90" t="s">
         <v>201</v>
       </c>
       <c r="E26" t="s">
@@ -6907,7 +6910,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="D27" s="94" t="s">
+      <c r="D27" s="90" t="s">
         <v>202</v>
       </c>
       <c r="E27" t="s">
@@ -6921,7 +6924,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="D28" s="91" t="s">
+      <c r="D28" s="88" t="s">
         <v>203</v>
       </c>
       <c r="E28" t="s">
@@ -6935,7 +6938,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="D29" s="91" t="s">
+      <c r="D29" s="88" t="s">
         <v>204</v>
       </c>
       <c r="E29" t="s">
@@ -6949,7 +6952,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="D30" s="91" t="s">
+      <c r="D30" s="88" t="s">
         <v>205</v>
       </c>
       <c r="E30" t="s">
@@ -6963,7 +6966,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="D31" s="91" t="s">
+      <c r="D31" s="88" t="s">
         <v>206</v>
       </c>
       <c r="E31" t="s">
@@ -6977,7 +6980,7 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="D32" s="91" t="s">
+      <c r="D32" s="88" t="s">
         <v>207</v>
       </c>
       <c r="G32" s="29">
@@ -6988,7 +6991,7 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="D33" s="91" t="s">
+      <c r="D33" s="88" t="s">
         <v>208</v>
       </c>
       <c r="G33" s="29">
@@ -7012,8 +7015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7081,7 +7084,7 @@
       <c r="A5" s="29">
         <v>1</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="100" t="s">
         <v>242</v>
       </c>
       <c r="E5" t="s">
@@ -7101,7 +7104,7 @@
       <c r="A6" s="29">
         <v>2</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="101" t="s">
         <v>243</v>
       </c>
       <c r="E6" t="s">
@@ -7121,7 +7124,7 @@
       <c r="A7" s="29">
         <v>3</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="101" t="s">
         <v>244</v>
       </c>
       <c r="E7" t="s">
@@ -7141,7 +7144,7 @@
       <c r="A8" s="29">
         <v>4</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="101" t="s">
         <v>245</v>
       </c>
       <c r="E8" t="s">
@@ -7161,7 +7164,7 @@
       <c r="A9" s="29">
         <v>5</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="101" t="s">
         <v>246</v>
       </c>
       <c r="E9" t="s">
@@ -7181,7 +7184,7 @@
       <c r="A10" s="29">
         <v>6</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="101" t="s">
         <v>247</v>
       </c>
       <c r="E10" t="s">
@@ -7201,7 +7204,7 @@
       <c r="A11" s="29">
         <v>7</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="101" t="s">
         <v>248</v>
       </c>
       <c r="E11" t="s">
@@ -7221,7 +7224,7 @@
       <c r="A12" s="29">
         <v>8</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="101" t="s">
         <v>249</v>
       </c>
       <c r="E12" t="s">
@@ -7241,7 +7244,7 @@
       <c r="A13" s="29">
         <v>9</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="101" t="s">
         <v>250</v>
       </c>
       <c r="E13" t="s">
@@ -7267,7 +7270,7 @@
       <c r="A14" s="29">
         <v>10</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="102" t="s">
         <v>251</v>
       </c>
       <c r="E14" t="s">
@@ -7290,7 +7293,7 @@
       <c r="A15" s="29">
         <v>11</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="39" t="s">
         <v>252</v>
       </c>
       <c r="E15" t="s">
@@ -7313,7 +7316,7 @@
       <c r="A16" s="29">
         <v>12</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="39" t="s">
         <v>253</v>
       </c>
       <c r="E16" t="s">
@@ -7336,7 +7339,7 @@
       <c r="A17" s="29">
         <v>13</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="39" t="s">
         <v>254</v>
       </c>
       <c r="E17" t="s">
@@ -7359,7 +7362,7 @@
       <c r="A18" s="29">
         <v>14</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="39" t="s">
         <v>255</v>
       </c>
       <c r="E18" t="s">
@@ -7382,7 +7385,7 @@
       <c r="A19" s="29">
         <v>15</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="39" t="s">
         <v>256</v>
       </c>
       <c r="E19" t="s">
@@ -7408,7 +7411,7 @@
       <c r="A20" s="29">
         <v>16</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="39" t="s">
         <v>257</v>
       </c>
       <c r="E20" t="s">
@@ -7428,7 +7431,7 @@
       <c r="A21" s="29">
         <v>17</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="39" t="s">
         <v>258</v>
       </c>
       <c r="E21" t="s">
@@ -7445,7 +7448,7 @@
       <c r="A22" s="29">
         <v>18</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="39" t="s">
         <v>210</v>
       </c>
       <c r="E22" t="s">
@@ -7459,7 +7462,7 @@
       <c r="A23" s="29">
         <v>19</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="39" t="s">
         <v>259</v>
       </c>
       <c r="E23" t="s">
@@ -7473,7 +7476,7 @@
       <c r="A24" s="29">
         <v>20</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="39" t="s">
         <v>260</v>
       </c>
       <c r="E24" t="s">
@@ -7484,7 +7487,7 @@
       <c r="A25" s="29">
         <v>21</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="39" t="s">
         <v>261</v>
       </c>
       <c r="E25" t="s">
@@ -7495,7 +7498,7 @@
       <c r="A26" s="29">
         <v>22</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="39" t="s">
         <v>262</v>
       </c>
       <c r="E26" t="s">
@@ -7506,7 +7509,7 @@
       <c r="A27" s="29">
         <v>23</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="39" t="s">
         <v>263</v>
       </c>
       <c r="E27" t="s">
@@ -7517,7 +7520,7 @@
       <c r="A28" s="29">
         <v>24</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="39" t="s">
         <v>264</v>
       </c>
       <c r="E28" t="s">
@@ -7528,7 +7531,7 @@
       <c r="A29" s="29">
         <v>25</v>
       </c>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="40" t="s">
         <v>211</v>
       </c>
       <c r="E29" t="s">
@@ -7536,12 +7539,12 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:11" s="97" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A32" s="96"/>
-      <c r="D32" s="98" t="s">
+    <row r="32" spans="1:11" s="93" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A32" s="92"/>
+      <c r="D32" s="94" t="s">
         <v>510</v>
       </c>
-      <c r="G32" s="99"/>
+      <c r="G32" s="95"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D34" s="16" t="s">
@@ -7681,8 +7684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7742,7 +7745,7 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="96" t="s">
         <v>212</v>
       </c>
       <c r="F4" t="s">
@@ -7756,7 +7759,7 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="101" t="s">
+      <c r="D5" s="96" t="s">
         <v>213</v>
       </c>
       <c r="F5" t="s">
@@ -7770,7 +7773,7 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="101" t="s">
+      <c r="D6" s="96" t="s">
         <v>214</v>
       </c>
       <c r="F6" t="s">
@@ -7784,7 +7787,7 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="101" t="s">
+      <c r="D7" s="96" t="s">
         <v>215</v>
       </c>
       <c r="F7" t="s">
@@ -7798,7 +7801,7 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="96" t="s">
         <v>216</v>
       </c>
       <c r="F8" t="s">
@@ -7812,7 +7815,7 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="101" t="s">
+      <c r="D9" s="96" t="s">
         <v>217</v>
       </c>
       <c r="F9" t="s">
@@ -7840,7 +7843,7 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="101" t="s">
+      <c r="D11" s="96" t="s">
         <v>219</v>
       </c>
       <c r="F11" t="s">
@@ -7854,7 +7857,7 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="101" t="s">
+      <c r="D12" s="96" t="s">
         <v>220</v>
       </c>
       <c r="F12" t="s">
@@ -7868,7 +7871,7 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="101" t="s">
+      <c r="D13" s="96" t="s">
         <v>221</v>
       </c>
       <c r="F13" t="s">
@@ -7882,7 +7885,7 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="96" t="s">
         <v>222</v>
       </c>
     </row>
@@ -7890,7 +7893,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="83" t="s">
         <v>223</v>
       </c>
     </row>
@@ -7898,7 +7901,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="86" t="s">
+      <c r="D16" s="83" t="s">
         <v>224</v>
       </c>
     </row>
@@ -7906,7 +7909,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="86" t="s">
+      <c r="D17" s="83" t="s">
         <v>225</v>
       </c>
     </row>
@@ -7914,7 +7917,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="83" t="s">
         <v>226</v>
       </c>
     </row>
@@ -7922,7 +7925,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="83" t="s">
         <v>227</v>
       </c>
     </row>
@@ -7930,7 +7933,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="86" t="s">
+      <c r="D20" s="83" t="s">
         <v>228</v>
       </c>
     </row>
@@ -7938,7 +7941,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="86" t="s">
+      <c r="D21" s="83" t="s">
         <v>229</v>
       </c>
     </row>
@@ -7946,7 +7949,7 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="D22" s="86" t="s">
+      <c r="D22" s="83" t="s">
         <v>230</v>
       </c>
     </row>
@@ -7954,7 +7957,7 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="D23" s="86" t="s">
+      <c r="D23" s="83" t="s">
         <v>231</v>
       </c>
     </row>
@@ -7962,7 +7965,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="D24" s="102" t="s">
+      <c r="D24" s="97" t="s">
         <v>232</v>
       </c>
     </row>
@@ -7970,7 +7973,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="D25" s="102" t="s">
+      <c r="D25" s="97" t="s">
         <v>233</v>
       </c>
     </row>
@@ -7978,7 +7981,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="D26" s="102" t="s">
+      <c r="D26" s="97" t="s">
         <v>234</v>
       </c>
     </row>
@@ -7986,7 +7989,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="D27" s="102" t="s">
+      <c r="D27" s="97" t="s">
         <v>235</v>
       </c>
     </row>
@@ -7994,7 +7997,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="D28" s="102" t="s">
+      <c r="D28" s="97" t="s">
         <v>236</v>
       </c>
     </row>
@@ -8002,7 +8005,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="D29" s="102" t="s">
+      <c r="D29" s="97" t="s">
         <v>237</v>
       </c>
     </row>
@@ -8010,7 +8013,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="D30" s="102" t="s">
+      <c r="D30" s="97" t="s">
         <v>238</v>
       </c>
     </row>
@@ -8018,7 +8021,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="D31" s="102" t="s">
+      <c r="D31" s="97" t="s">
         <v>239</v>
       </c>
     </row>
@@ -8026,7 +8029,7 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="D32" s="102" t="s">
+      <c r="D32" s="97" t="s">
         <v>240</v>
       </c>
     </row>
@@ -8034,7 +8037,7 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="D33" s="102" t="s">
+      <c r="D33" s="97" t="s">
         <v>241</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   20-05-2021 - 21:15:05.22
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="526">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2403,14 +2403,14 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="8" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="8" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="8" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="14" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -6241,8 +6241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6265,15 +6265,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="73" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="103" t="s">
         <v>350</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
       <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6756,7 +6756,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="103" t="s">
+      <c r="D16" s="102" t="s">
         <v>191</v>
       </c>
       <c r="E16" t="s">
@@ -6770,7 +6770,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="103" t="s">
+      <c r="D17" s="102" t="s">
         <v>192</v>
       </c>
       <c r="E17" t="s">
@@ -6784,7 +6784,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="103" t="s">
+      <c r="D18" s="102" t="s">
         <v>193</v>
       </c>
       <c r="E18" t="s">
@@ -6798,7 +6798,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="103" t="s">
+      <c r="D19" s="102" t="s">
         <v>194</v>
       </c>
       <c r="E19" t="s">
@@ -7015,8 +7015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7084,7 +7084,7 @@
       <c r="A5" s="29">
         <v>1</v>
       </c>
-      <c r="D5" s="100" t="s">
+      <c r="D5" s="99" t="s">
         <v>242</v>
       </c>
       <c r="E5" t="s">
@@ -7104,7 +7104,7 @@
       <c r="A6" s="29">
         <v>2</v>
       </c>
-      <c r="D6" s="101" t="s">
+      <c r="D6" s="100" t="s">
         <v>243</v>
       </c>
       <c r="E6" t="s">
@@ -7124,7 +7124,7 @@
       <c r="A7" s="29">
         <v>3</v>
       </c>
-      <c r="D7" s="101" t="s">
+      <c r="D7" s="100" t="s">
         <v>244</v>
       </c>
       <c r="E7" t="s">
@@ -7144,7 +7144,7 @@
       <c r="A8" s="29">
         <v>4</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="100" t="s">
         <v>245</v>
       </c>
       <c r="E8" t="s">
@@ -7164,7 +7164,7 @@
       <c r="A9" s="29">
         <v>5</v>
       </c>
-      <c r="D9" s="101" t="s">
+      <c r="D9" s="100" t="s">
         <v>246</v>
       </c>
       <c r="E9" t="s">
@@ -7184,7 +7184,7 @@
       <c r="A10" s="29">
         <v>6</v>
       </c>
-      <c r="D10" s="101" t="s">
+      <c r="D10" s="100" t="s">
         <v>247</v>
       </c>
       <c r="E10" t="s">
@@ -7204,7 +7204,7 @@
       <c r="A11" s="29">
         <v>7</v>
       </c>
-      <c r="D11" s="101" t="s">
+      <c r="D11" s="100" t="s">
         <v>248</v>
       </c>
       <c r="E11" t="s">
@@ -7224,7 +7224,7 @@
       <c r="A12" s="29">
         <v>8</v>
       </c>
-      <c r="D12" s="101" t="s">
+      <c r="D12" s="100" t="s">
         <v>249</v>
       </c>
       <c r="E12" t="s">
@@ -7244,7 +7244,7 @@
       <c r="A13" s="29">
         <v>9</v>
       </c>
-      <c r="D13" s="101" t="s">
+      <c r="D13" s="100" t="s">
         <v>250</v>
       </c>
       <c r="E13" t="s">
@@ -7270,7 +7270,7 @@
       <c r="A14" s="29">
         <v>10</v>
       </c>
-      <c r="D14" s="102" t="s">
+      <c r="D14" s="101" t="s">
         <v>251</v>
       </c>
       <c r="E14" t="s">
@@ -7437,6 +7437,12 @@
       <c r="E21" t="s">
         <v>33</v>
       </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
       <c r="H21" s="16" t="s">
         <v>505</v>
       </c>
@@ -7453,6 +7459,12 @@
       </c>
       <c r="E22" t="s">
         <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>517</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   20-05-2021 - 23:08:53.00
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="526">
   <si>
     <t>TOPIC</t>
   </si>
@@ -7016,7 +7016,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7480,6 +7480,12 @@
       <c r="E23" t="s">
         <v>33</v>
       </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
       <c r="K23" s="16" t="s">
         <v>525</v>
       </c>
@@ -7494,6 +7500,12 @@
       <c r="E24" t="s">
         <v>33</v>
       </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
@@ -7505,6 +7517,12 @@
       <c r="E25" t="s">
         <v>33</v>
       </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
@@ -7515,6 +7533,12 @@
       </c>
       <c r="E26" t="s">
         <v>33</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code on timestamp:   21-05-2021 -  0:00:00.94
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="529">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1780,6 +1780,18 @@
   </si>
   <si>
     <t>CP/KReverseinLL.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>go to mid 
+reverse</t>
+  </si>
+  <si>
+    <t>go to mid
+reverse
+equivalent to palindrome</t>
+  </si>
+  <si>
+    <t>you are given only head and performing operation</t>
   </si>
 </sst>
 </file>
@@ -3848,7 +3860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -4809,7 +4821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -5340,7 +5352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
@@ -6241,7 +6253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -6528,7 +6540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20:D23"/>
     </sheetView>
   </sheetViews>
@@ -7015,8 +7027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7524,7 +7536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>22</v>
       </c>
@@ -7540,8 +7552,11 @@
       <c r="G26" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H26" s="18" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>23</v>
       </c>
@@ -7550,6 +7565,18 @@
       </c>
       <c r="E27" t="s">
         <v>33</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>527</v>
+      </c>
+      <c r="I27" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code on timestamp:   21-05-2021 -  0:52:21.68
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="530">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1792,6 +1792,9 @@
   </si>
   <si>
     <t>you are given only head and performing operation</t>
+  </si>
+  <si>
+    <t>check video how to manage tail using prev rather than using loop of n</t>
   </si>
 </sst>
 </file>
@@ -7575,8 +7578,11 @@
       <c r="H27" s="18" t="s">
         <v>527</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="18" t="s">
         <v>528</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code on timestamp:   21-05-2021 - 22:28:56.32
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="534">
   <si>
     <t>TOPIC</t>
   </si>
@@ -428,9 +428,6 @@
   </si>
   <si>
     <t xml:space="preserve">char to number </t>
-  </si>
-  <si>
-    <t>number to char</t>
   </si>
   <si>
     <t>Ascii</t>
@@ -1795,6 +1792,21 @@
   </si>
   <si>
     <t>check video how to manage tail using prev rather than using loop of n</t>
+  </si>
+  <si>
+    <t>number to char(letter)</t>
+  </si>
+  <si>
+    <t>number to char(number)</t>
+  </si>
+  <si>
+    <t>5+'0' =="5"</t>
+  </si>
+  <si>
+    <t>Find and Replace Pattern - LeetCode</t>
+  </si>
+  <si>
+    <t>pattern matching with index</t>
   </si>
 </sst>
 </file>
@@ -2464,13 +2476,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>33651</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2764,10 +2776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J17"/>
+  <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2785,10 +2797,10 @@
         <v>120</v>
       </c>
       <c r="G2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -2796,7 +2808,7 @@
         <v>121</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2805,60 +2817,69 @@
         <v>48</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>122</v>
+        <v>530</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="F4" t="s">
+        <v>531</v>
+      </c>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>529</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5">
+        <v>97</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>392</v>
+      </c>
+      <c r="F6" t="s">
         <v>124</v>
       </c>
-      <c r="G4">
-        <v>97</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>393</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
         <v>125</v>
       </c>
-      <c r="G5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G6">
+      <c r="G7">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E16" s="12"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" display="https://www.geeksforgeeks.org/java-tricks-competitive-programming-java-8/"/>
-    <hyperlink ref="J4" r:id="rId2" display="https://www.geeksforgeeks.org/fast-io-in-java-in-competitive-programming/"/>
+    <hyperlink ref="J5" r:id="rId2" display="https://www.geeksforgeeks.org/fast-io-in-java-in-competitive-programming/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2912,7 +2933,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -2932,7 +2953,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="96" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2940,7 +2961,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2948,7 +2969,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="96" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2956,7 +2977,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="96" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2964,7 +2985,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="96" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2972,7 +2993,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="96" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2980,7 +3001,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="96" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2988,7 +3009,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="96" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2996,7 +3017,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="96" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3004,7 +3025,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="96" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3012,7 +3033,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="83" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3020,7 +3041,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3028,7 +3049,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="83" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3036,7 +3057,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3044,7 +3065,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="83" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3052,7 +3073,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="83" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3060,7 +3081,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="83" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3068,7 +3089,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="83" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3076,7 +3097,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="83" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3084,7 +3105,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="83" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3136,7 +3157,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3156,7 +3177,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="98" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3164,7 +3185,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="98" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3172,7 +3193,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="98" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3180,7 +3201,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="98" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3188,7 +3209,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="98" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3196,7 +3217,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="98" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3204,7 +3225,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="98" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3212,7 +3233,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="98" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3220,7 +3241,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="98" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3228,7 +3249,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="98" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -3280,7 +3301,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3300,7 +3321,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="96" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3308,7 +3329,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3316,7 +3337,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="96" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3324,7 +3345,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="96" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3332,7 +3353,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="96" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3340,7 +3361,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="96" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3348,7 +3369,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="96" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3356,7 +3377,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="96" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3364,7 +3385,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="96" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3372,7 +3393,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="96" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3380,7 +3401,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="83" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3388,7 +3409,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3396,7 +3417,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="83" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3404,7 +3425,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -3459,7 +3480,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3479,7 +3500,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="96" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3487,7 +3508,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3495,7 +3516,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="96" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3503,7 +3524,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="96" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3511,7 +3532,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="96" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3519,7 +3540,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="96" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3527,7 +3548,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="96" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3535,7 +3556,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="96" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3543,7 +3564,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="96" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3551,7 +3572,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="96" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3559,7 +3580,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="83" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3567,7 +3588,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3575,7 +3596,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="83" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3583,7 +3604,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3591,7 +3612,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="83" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3599,7 +3620,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="83" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3607,7 +3628,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="83" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3615,7 +3636,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="83" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -3627,8 +3648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3646,16 +3667,16 @@
         <v>51</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>38</v>
@@ -3672,13 +3693,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="16" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3686,21 +3707,21 @@
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="16" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J6" s="10"/>
     </row>
@@ -3709,11 +3730,11 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="16" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -3722,7 +3743,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="10"/>
       <c r="I7" s="16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -3731,24 +3752,24 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="80" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>477</v>
-      </c>
       <c r="I8" s="16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J8" s="10"/>
     </row>
@@ -3757,43 +3778,48 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="16" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G9" s="91" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="16" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D10" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="G10" t="s">
         <v>498</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" s="16" t="s">
         <v>499</v>
       </c>
-      <c r="I10" s="16" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="31"/>
+      <c r="D11" s="16" t="s">
+        <v>532</v>
+      </c>
+      <c r="F11" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="31"/>
@@ -3853,9 +3879,10 @@
     <hyperlink ref="I9" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/Leet_longest_string_chain_Recursive_approach.java"/>
     <hyperlink ref="D10" r:id="rId10" display="https://leetcode.com/problems/coin-change/"/>
     <hyperlink ref="I10" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/Leet_coinchange.java"/>
+    <hyperlink ref="D11" r:id="rId12" display="https://leetcode.com/problems/find-and-replace-pattern/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -3914,7 +3941,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>38</v>
@@ -3923,7 +3950,7 @@
         <v>37</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>74</v>
@@ -4213,7 +4240,7 @@
         <v>97</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>96</v>
@@ -4242,10 +4269,10 @@
         <v>100</v>
       </c>
       <c r="I14" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="J14" s="10" t="s">
         <v>435</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>436</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>98</v>
@@ -4274,7 +4301,7 @@
         <v>100</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -4300,7 +4327,7 @@
         <v>100</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4326,10 +4353,10 @@
         <v>100</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4705,7 +4732,7 @@
         <v>101</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K31" s="16"/>
     </row>
@@ -4717,7 +4744,7 @@
         <v>32</v>
       </c>
       <c r="D32" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>33</v>
@@ -4729,25 +4756,25 @@
         <v>2</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K32" s="16"/>
     </row>
     <row r="33" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G33" s="2">
         <v>2</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K33" s="16"/>
     </row>
@@ -4771,13 +4798,13 @@
         <v>2</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>63</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K34" s="16"/>
     </row>
@@ -4848,7 +4875,7 @@
         <v>116</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -4882,7 +4909,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -4899,7 +4926,7 @@
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D4" s="25" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K4" s="16"/>
     </row>
@@ -4926,7 +4953,7 @@
         <v>105</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4952,7 +4979,7 @@
         <v>71</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -4972,7 +4999,7 @@
         <v>67</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -4980,7 +5007,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="84" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>34</v>
@@ -4989,13 +5016,13 @@
         <v>2</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -5003,16 +5030,16 @@
         <v>5</v>
       </c>
       <c r="D10" s="84" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G10" s="5">
         <v>0</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5020,7 +5047,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="84" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F11" s="79" t="s">
         <v>34</v>
@@ -5029,10 +5056,10 @@
         <v>2</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -5040,7 +5067,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="84" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>34</v>
@@ -5049,10 +5076,10 @@
         <v>3</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -5060,7 +5087,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="84" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>34</v>
@@ -5069,16 +5096,16 @@
         <v>2</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -5086,7 +5113,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>34</v>
@@ -5095,16 +5122,16 @@
         <v>2</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5112,10 +5139,10 @@
         <v>10</v>
       </c>
       <c r="C15" s="81" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>34</v>
@@ -5124,16 +5151,16 @@
         <v>2</v>
       </c>
       <c r="H15" s="15" t="s">
+        <v>477</v>
+      </c>
+      <c r="I15" s="15" t="s">
         <v>478</v>
       </c>
-      <c r="I15" s="15" t="s">
-        <v>479</v>
-      </c>
       <c r="J15" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -5141,7 +5168,7 @@
         <v>11</v>
       </c>
       <c r="D16" s="82" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>34</v>
@@ -5150,13 +5177,13 @@
         <v>2</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -5164,7 +5191,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="84" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>34</v>
@@ -5173,13 +5200,13 @@
         <v>2</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="195" x14ac:dyDescent="0.25">
@@ -5187,7 +5214,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="84" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>34</v>
@@ -5196,13 +5223,13 @@
         <v>2</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -5210,22 +5237,22 @@
         <v>14</v>
       </c>
       <c r="D19" s="84" t="s">
+        <v>159</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="G19" s="5">
         <v>2</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -5233,7 +5260,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>34</v>
@@ -5242,10 +5269,10 @@
         <v>2</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -5253,7 +5280,7 @@
         <v>16</v>
       </c>
       <c r="D21" s="84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>34</v>
@@ -5262,10 +5289,10 @@
         <v>2</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -5273,7 +5300,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="84" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>34</v>
@@ -5282,10 +5309,10 @@
         <v>2</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -5293,10 +5320,10 @@
         <v>18</v>
       </c>
       <c r="D23" s="85" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -5304,7 +5331,7 @@
         <v>19</v>
       </c>
       <c r="D24" s="85" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5315,7 +5342,7 @@
         <v>20</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5323,7 +5350,7 @@
         <v>21</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -5378,17 +5405,17 @@
         <v>116</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I1"/>
     </row>
     <row r="2" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32"/>
       <c r="B2" s="38" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="32"/>
@@ -5412,7 +5439,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>38</v>
@@ -5444,13 +5471,13 @@
         <v>5</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.25">
@@ -5470,13 +5497,13 @@
         <v>5</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -5484,7 +5511,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>33</v>
@@ -5496,13 +5523,13 @@
         <v>5</v>
       </c>
       <c r="F6" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>339</v>
-      </c>
       <c r="I6" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -5522,13 +5549,13 @@
         <v>5</v>
       </c>
       <c r="G7" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>340</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5548,10 +5575,10 @@
         <v>5</v>
       </c>
       <c r="G8" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="I8" s="16" t="s">
         <v>342</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5571,10 +5598,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>351</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -5594,16 +5621,16 @@
         <v>3</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -5623,13 +5650,13 @@
         <v>3</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5649,13 +5676,13 @@
         <v>3</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5675,13 +5702,13 @@
         <v>3</v>
       </c>
       <c r="F13" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="G13" s="10" t="s">
-        <v>370</v>
-      </c>
       <c r="I13" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -5701,13 +5728,13 @@
         <v>3</v>
       </c>
       <c r="G14" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>402</v>
-      </c>
       <c r="I14" s="16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5727,10 +5754,10 @@
         <v>3</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5750,10 +5777,10 @@
         <v>3</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5773,10 +5800,10 @@
         <v>3</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -5796,7 +5823,7 @@
         <v>3</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5816,16 +5843,16 @@
         <v>3</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5845,10 +5872,10 @@
         <v>3</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -5863,7 +5890,7 @@
     <row r="32" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32"/>
       <c r="B32" s="38" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="32"/>
@@ -5878,19 +5905,19 @@
         <v>1</v>
       </c>
       <c r="B33" s="31" t="s">
+        <v>346</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="10" t="s">
         <v>347</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>348</v>
       </c>
       <c r="I33" s="31"/>
     </row>
@@ -5899,10 +5926,10 @@
         <v>2</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>34</v>
@@ -5911,10 +5938,10 @@
         <v>0</v>
       </c>
       <c r="F34" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="G34" s="10" t="s">
         <v>354</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>355</v>
       </c>
       <c r="I34" s="31"/>
     </row>
@@ -5923,7 +5950,7 @@
         <v>3</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>33</v>
@@ -5935,7 +5962,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I35" s="31"/>
     </row>
@@ -5944,22 +5971,22 @@
         <v>4</v>
       </c>
       <c r="B36" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="2">
-        <v>0</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>358</v>
-      </c>
       <c r="G36" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H36" s="60"/>
       <c r="I36" s="31"/>
@@ -5969,11 +5996,11 @@
         <v>5</v>
       </c>
       <c r="B37" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>357</v>
-      </c>
       <c r="D37" s="5" t="s">
         <v>34</v>
       </c>
@@ -5981,7 +6008,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H37" s="60"/>
       <c r="I37" s="31"/>
@@ -5991,22 +6018,22 @@
         <v>6</v>
       </c>
       <c r="B38" s="31" t="s">
+        <v>359</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="2">
-        <v>0</v>
-      </c>
-      <c r="F38" s="10" t="s">
+      <c r="G38" s="10" t="s">
         <v>361</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>362</v>
       </c>
       <c r="I38" s="31"/>
     </row>
@@ -6015,10 +6042,10 @@
         <v>7</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>34</v>
@@ -6027,7 +6054,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I39" s="31"/>
     </row>
@@ -6036,10 +6063,10 @@
         <v>8</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>34</v>
@@ -6048,10 +6075,10 @@
         <v>0</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I40" s="31"/>
     </row>
@@ -6060,22 +6087,22 @@
         <v>9</v>
       </c>
       <c r="B41" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="G41" s="10" t="s">
         <v>379</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="2">
-        <v>0</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>381</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>380</v>
       </c>
       <c r="I41" s="31"/>
     </row>
@@ -6084,22 +6111,22 @@
         <v>10</v>
       </c>
       <c r="B42" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
+      </c>
+      <c r="F42" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="2">
-        <v>0</v>
-      </c>
-      <c r="F42" s="10" t="s">
+      <c r="G42" s="10" t="s">
         <v>383</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>384</v>
       </c>
       <c r="I42" s="31"/>
     </row>
@@ -6108,25 +6135,25 @@
         <v>11</v>
       </c>
       <c r="B43" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H43" s="10" t="s">
         <v>385</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="2">
-        <v>0</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>387</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>386</v>
       </c>
       <c r="I43" s="31"/>
     </row>
@@ -6135,25 +6162,25 @@
         <v>12</v>
       </c>
       <c r="B44" s="21" t="s">
+        <v>389</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+      <c r="F44" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E44" s="2">
-        <v>0</v>
-      </c>
-      <c r="F44" s="10" t="s">
+      <c r="G44" s="10" t="s">
         <v>391</v>
       </c>
-      <c r="G44" s="10" t="s">
-        <v>392</v>
-      </c>
       <c r="H44" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I44" s="21"/>
     </row>
@@ -6162,22 +6189,22 @@
         <v>13</v>
       </c>
       <c r="B45" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0</v>
+      </c>
+      <c r="F45" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="2">
-        <v>0</v>
-      </c>
-      <c r="F45" s="10" t="s">
+      <c r="G45" s="10" t="s">
         <v>395</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>396</v>
       </c>
       <c r="I45" s="16"/>
     </row>
@@ -6186,25 +6213,25 @@
         <v>14</v>
       </c>
       <c r="B46" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="H46" s="10" t="s">
         <v>397</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -6275,13 +6302,13 @@
         <v>116</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="73" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A2" s="103" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B2" s="103"/>
       <c r="C2" s="103"/>
@@ -6305,7 +6332,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>38</v>
@@ -6325,7 +6352,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="77" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>33</v>
@@ -6337,12 +6364,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="11"/>
       <c r="I4" s="16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -6359,7 +6386,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="11"/>
       <c r="I5" s="16" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -6382,7 +6409,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
       <c r="I6" s="16" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6405,7 +6432,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
       <c r="I7" s="16" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6428,7 +6455,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
       <c r="I8" s="16" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -6451,7 +6478,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="11"/>
       <c r="I9" s="16" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6472,11 +6499,11 @@
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="78" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="16" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6484,36 +6511,36 @@
         <v>8</v>
       </c>
       <c r="B11" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>409</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="75" t="s">
+        <v>409</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>411</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -6584,7 +6611,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -6604,7 +6631,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="86" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
         <v>33</v>
@@ -6618,7 +6645,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="86" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
@@ -6632,7 +6659,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="86" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6" t="s">
         <v>33</v>
@@ -6646,7 +6673,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="86" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -6660,7 +6687,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="86" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
@@ -6674,7 +6701,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="86" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -6688,10 +6715,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="87" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G10" s="29">
         <v>0</v>
@@ -6702,7 +6729,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="87" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
@@ -6716,10 +6743,10 @@
         <v>9</v>
       </c>
       <c r="D12" s="87" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G12" s="29">
         <v>0</v>
@@ -6730,7 +6757,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="87" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -6744,7 +6771,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="87" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -6758,7 +6785,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="87" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E15" t="s">
         <v>33</v>
@@ -6772,7 +6799,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="102" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
@@ -6786,7 +6813,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="102" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
@@ -6800,7 +6827,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="102" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E18" t="s">
         <v>33</v>
@@ -6814,7 +6841,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="102" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E19" t="s">
         <v>33</v>
@@ -6828,7 +6855,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="89" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
@@ -6842,7 +6869,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="89" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
@@ -6856,7 +6883,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="89" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
@@ -6870,7 +6897,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="89" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -6884,7 +6911,7 @@
         <v>21</v>
       </c>
       <c r="D24" s="90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -6898,7 +6925,7 @@
         <v>22</v>
       </c>
       <c r="D25" s="90" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -6912,7 +6939,7 @@
         <v>23</v>
       </c>
       <c r="D26" s="90" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E26" t="s">
         <v>33</v>
@@ -6926,7 +6953,7 @@
         <v>24</v>
       </c>
       <c r="D27" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
@@ -6940,7 +6967,7 @@
         <v>25</v>
       </c>
       <c r="D28" s="88" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E28" t="s">
         <v>33</v>
@@ -6954,7 +6981,7 @@
         <v>26</v>
       </c>
       <c r="D29" s="88" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E29" t="s">
         <v>33</v>
@@ -6968,10 +6995,10 @@
         <v>27</v>
       </c>
       <c r="D30" s="88" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G30" s="29">
         <v>0</v>
@@ -6982,10 +7009,10 @@
         <v>28</v>
       </c>
       <c r="D31" s="88" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G31" s="29">
         <v>0</v>
@@ -6996,7 +7023,7 @@
         <v>29</v>
       </c>
       <c r="D32" s="88" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G32" s="29">
         <v>0</v>
@@ -7007,7 +7034,7 @@
         <v>30</v>
       </c>
       <c r="D33" s="88" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G33" s="29">
         <v>0</v>
@@ -7015,7 +7042,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -7030,7 +7057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -7075,7 +7102,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -7092,7 +7119,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K4" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -7100,7 +7127,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="99" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
@@ -7112,7 +7139,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7120,7 +7147,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="100" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E6" t="s">
         <v>33</v>
@@ -7132,7 +7159,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -7140,7 +7167,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="100" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -7152,7 +7179,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -7160,7 +7187,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="100" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
@@ -7172,7 +7199,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -7180,7 +7207,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="100" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -7192,7 +7219,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -7200,7 +7227,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="100" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -7212,7 +7239,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -7220,7 +7247,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="100" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
@@ -7232,7 +7259,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -7240,7 +7267,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="100" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
@@ -7252,7 +7279,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -7260,7 +7287,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="100" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -7272,13 +7299,13 @@
         <v>1</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7286,7 +7313,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="101" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -7298,10 +7325,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -7309,7 +7336,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E15" t="s">
         <v>33</v>
@@ -7321,10 +7348,10 @@
         <v>1</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -7332,7 +7359,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
@@ -7344,10 +7371,10 @@
         <v>1</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7355,7 +7382,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
@@ -7367,10 +7394,10 @@
         <v>1</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -7378,7 +7405,7 @@
         <v>14</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E18" t="s">
         <v>33</v>
@@ -7390,10 +7417,10 @@
         <v>1</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -7401,7 +7428,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E19" t="s">
         <v>33</v>
@@ -7413,13 +7440,13 @@
         <v>0</v>
       </c>
       <c r="H19" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="I19" t="s">
+        <v>502</v>
+      </c>
+      <c r="K19" s="16" t="s">
         <v>501</v>
-      </c>
-      <c r="I19" t="s">
-        <v>503</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -7427,7 +7454,7 @@
         <v>16</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
@@ -7439,7 +7466,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -7447,7 +7474,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
@@ -7459,10 +7486,10 @@
         <v>0</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -7470,7 +7497,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
@@ -7482,7 +7509,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -7490,7 +7517,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -7502,7 +7529,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -7510,7 +7537,7 @@
         <v>20</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -7527,7 +7554,7 @@
         <v>21</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -7544,7 +7571,7 @@
         <v>22</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E26" t="s">
         <v>33</v>
@@ -7556,7 +7583,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -7564,7 +7591,7 @@
         <v>23</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
@@ -7576,13 +7603,13 @@
         <v>0</v>
       </c>
       <c r="H27" s="18" t="s">
+        <v>526</v>
+      </c>
+      <c r="I27" s="18" t="s">
         <v>527</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="J27" s="18" t="s">
         <v>528</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -7590,7 +7617,7 @@
         <v>24</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E28" t="s">
         <v>33</v>
@@ -7601,7 +7628,7 @@
         <v>25</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E29" t="s">
         <v>33</v>
@@ -7611,13 +7638,13 @@
     <row r="32" spans="1:11" s="93" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A32" s="92"/>
       <c r="D32" s="94" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G32" s="95"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D34" s="16" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F34" t="s">
         <v>34</v>
@@ -7628,7 +7655,7 @@
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D35" s="16" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F35" t="s">
         <v>34</v>
@@ -7639,7 +7666,7 @@
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D36" s="16" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F36" t="s">
         <v>34</v>
@@ -7650,7 +7677,7 @@
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D37" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F37" t="s">
         <v>34</v>
@@ -7661,7 +7688,7 @@
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F38" t="s">
         <v>34</v>
@@ -7670,13 +7697,13 @@
         <v>0</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K38" s="16"/>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F39" t="s">
         <v>34</v>
@@ -7687,12 +7714,12 @@
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D40" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D41" s="16" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F41" t="s">
         <v>34</v>
@@ -7703,10 +7730,10 @@
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -7795,7 +7822,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -7815,7 +7842,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="96" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
@@ -7829,7 +7856,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -7843,7 +7870,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="96" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -7857,7 +7884,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="96" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
@@ -7871,7 +7898,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="96" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F8" t="s">
         <v>34</v>
@@ -7885,7 +7912,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="96" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F9" t="s">
         <v>34</v>
@@ -7899,7 +7926,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
@@ -7913,7 +7940,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="96" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F11" t="s">
         <v>34</v>
@@ -7927,7 +7954,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="96" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F12" t="s">
         <v>34</v>
@@ -7941,7 +7968,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="96" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
@@ -7955,7 +7982,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="96" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -7963,7 +7990,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -7971,7 +7998,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="83" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7979,7 +8006,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7987,7 +8014,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="83" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -7995,7 +8022,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="83" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -8003,7 +8030,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="83" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -8011,7 +8038,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="83" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -8019,7 +8046,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="83" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -8027,7 +8054,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="83" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -8035,7 +8062,7 @@
         <v>21</v>
       </c>
       <c r="D24" s="97" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -8043,7 +8070,7 @@
         <v>22</v>
       </c>
       <c r="D25" s="97" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -8051,7 +8078,7 @@
         <v>23</v>
       </c>
       <c r="D26" s="97" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -8059,7 +8086,7 @@
         <v>24</v>
       </c>
       <c r="D27" s="97" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -8067,7 +8094,7 @@
         <v>25</v>
       </c>
       <c r="D28" s="97" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -8075,7 +8102,7 @@
         <v>26</v>
       </c>
       <c r="D29" s="97" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -8083,7 +8110,7 @@
         <v>27</v>
       </c>
       <c r="D30" s="97" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -8091,7 +8118,7 @@
         <v>28</v>
       </c>
       <c r="D31" s="97" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8099,7 +8126,7 @@
         <v>29</v>
       </c>
       <c r="D32" s="97" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -8107,7 +8134,7 @@
         <v>30</v>
       </c>
       <c r="D33" s="97" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code on timestamp:   21-05-2021 - 22:36:56.67
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="536">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1807,6 +1807,12 @@
   </si>
   <si>
     <t>pattern matching with index</t>
+  </si>
+  <si>
+    <t>CP/Leet_890.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>leet</t>
   </si>
 </sst>
 </file>
@@ -3649,7 +3655,7 @@
   <dimension ref="A4:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3814,11 +3820,20 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C11" t="s">
+        <v>208</v>
+      </c>
       <c r="D11" s="16" t="s">
         <v>532</v>
       </c>
       <c r="F11" t="s">
         <v>533</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3880,9 +3895,10 @@
     <hyperlink ref="D10" r:id="rId10" display="https://leetcode.com/problems/coin-change/"/>
     <hyperlink ref="I10" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/Leet_coinchange.java"/>
     <hyperlink ref="D11" r:id="rId12" display="https://leetcode.com/problems/find-and-replace-pattern/"/>
+    <hyperlink ref="I11" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/3.leetcode-premium-master/LeetCode/Leet_890.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 -  1:07:42.34
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="540">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1783,36 +1783,49 @@
 reverse</t>
   </si>
   <si>
+    <t>you are given only head and performing operation</t>
+  </si>
+  <si>
+    <t>check video how to manage tail using prev rather than using loop of n</t>
+  </si>
+  <si>
+    <t>number to char(letter)</t>
+  </si>
+  <si>
+    <t>number to char(number)</t>
+  </si>
+  <si>
+    <t>5+'0' =="5"</t>
+  </si>
+  <si>
+    <t>Find and Replace Pattern - LeetCode</t>
+  </si>
+  <si>
+    <t>pattern matching with index</t>
+  </si>
+  <si>
+    <t>CP/Leet_890.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>leet</t>
+  </si>
+  <si>
+    <t>CP/DisplayReverseRecursive.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/ReverseLL_Pointer_Recursive.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/LL_palindrome_Or_note.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/FoldALL.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
     <t>go to mid
 reverse
+manage the references
 equivalent to palindrome</t>
-  </si>
-  <si>
-    <t>you are given only head and performing operation</t>
-  </si>
-  <si>
-    <t>check video how to manage tail using prev rather than using loop of n</t>
-  </si>
-  <si>
-    <t>number to char(letter)</t>
-  </si>
-  <si>
-    <t>number to char(number)</t>
-  </si>
-  <si>
-    <t>5+'0' =="5"</t>
-  </si>
-  <si>
-    <t>Find and Replace Pattern - LeetCode</t>
-  </si>
-  <si>
-    <t>pattern matching with index</t>
-  </si>
-  <si>
-    <t>CP/Leet_890.java at main · spartan4cs/CP (github.com)</t>
-  </si>
-  <si>
-    <t>leet</t>
   </si>
 </sst>
 </file>
@@ -2828,16 +2841,16 @@
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>529</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>530</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>531</v>
       </c>
       <c r="J4" s="16"/>
     </row>
     <row r="5" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>127</v>
@@ -3654,7 +3667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3821,19 +3834,19 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C11" t="s">
         <v>208</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>531</v>
+      </c>
+      <c r="F11" t="s">
         <v>532</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" s="16" t="s">
         <v>533</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -7073,8 +7086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7564,6 +7577,9 @@
       <c r="G24" s="5">
         <v>0</v>
       </c>
+      <c r="K24" s="16" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
@@ -7581,6 +7597,9 @@
       <c r="G25" s="5">
         <v>0</v>
       </c>
+      <c r="K25" s="16" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
@@ -7601,8 +7620,11 @@
       <c r="H26" s="18" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="K26" s="16" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>23</v>
       </c>
@@ -7619,13 +7641,16 @@
         <v>0</v>
       </c>
       <c r="H27" s="18" t="s">
+        <v>539</v>
+      </c>
+      <c r="I27" s="18" t="s">
         <v>526</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="J27" s="18" t="s">
         <v>527</v>
       </c>
-      <c r="J27" s="18" t="s">
-        <v>528</v>
+      <c r="K27" s="16" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -7787,6 +7812,10 @@
     <hyperlink ref="K13" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Iterative.java"/>
     <hyperlink ref="K14" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Pointer.java"/>
     <hyperlink ref="K23" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KReverseinLL.java"/>
+    <hyperlink ref="K24" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java"/>
+    <hyperlink ref="K25" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java"/>
+    <hyperlink ref="K26" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java"/>
+    <hyperlink ref="K27" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALL.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 -  1:14:12.62
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -1819,13 +1819,13 @@
     <t>CP/LL_palindrome_Or_note.java at main · spartan4cs/CP (github.com)</t>
   </si>
   <si>
-    <t>CP/FoldALL.java at main · spartan4cs/CP (github.com)</t>
-  </si>
-  <si>
     <t>go to mid
 reverse
 manage the references
 equivalent to palindrome</t>
+  </si>
+  <si>
+    <t>CP/FoldALinkedList.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -7086,8 +7086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7641,7 +7641,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I27" s="18" t="s">
         <v>526</v>
@@ -7650,7 +7650,7 @@
         <v>527</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -7815,7 +7815,7 @@
     <hyperlink ref="K24" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java"/>
     <hyperlink ref="K25" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java"/>
     <hyperlink ref="K26" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java"/>
-    <hyperlink ref="K27" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALL.java"/>
+    <hyperlink ref="K27" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 -  3:12:33.03
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="539">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1670,9 +1670,6 @@
     <t>CP/BaseCountSort.java at main · spartan4cs/CP (github.com)</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>RT</t>
   </si>
   <si>
@@ -1825,7 +1822,7 @@
 equivalent to palindrome</t>
   </si>
   <si>
-    <t>CP/FoldALinkedList.java at main · spartan4cs/CP (github.com)</t>
+    <t>CP/NGETR.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -2841,16 +2838,16 @@
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>528</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>529</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>530</v>
       </c>
       <c r="J4" s="16"/>
     </row>
     <row r="5" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>127</v>
@@ -2886,7 +2883,7 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
@@ -2952,7 +2949,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3176,7 +3173,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3320,7 +3317,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3499,7 +3496,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3686,7 +3683,7 @@
         <v>51</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
@@ -3695,7 +3692,7 @@
         <v>418</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>38</v>
@@ -3797,56 +3794,56 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="16" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G9" s="91" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="16" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D10" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="G10" t="s">
         <v>497</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" s="16" t="s">
         <v>498</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C11" t="s">
         <v>208</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="F11" t="s">
         <v>531</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" s="16" t="s">
         <v>532</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3919,7 +3916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -3970,7 +3967,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>38</v>
@@ -4938,7 +4935,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -5411,8 +5408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5468,7 +5465,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>38</v>
@@ -5558,7 +5555,7 @@
         <v>338</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>489</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -6260,7 +6257,7 @@
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -6285,23 +6282,23 @@
     <hyperlink ref="B48" r:id="rId18" display="https://leetcode.com/problems/merge-intervals/"/>
     <hyperlink ref="G1" r:id="rId19" display="https://github.com/spartan4cs/CP/tree/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues"/>
     <hyperlink ref="I4" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Duplicatebracket.java"/>
-    <hyperlink ref="I6" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java"/>
-    <hyperlink ref="I7" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/StockSpan.java"/>
-    <hyperlink ref="I8" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/LargestAreaHistogram.java"/>
-    <hyperlink ref="I9" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/SlidingWindowMax.java"/>
-    <hyperlink ref="I5" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/BalancedBracket.java"/>
-    <hyperlink ref="I14" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/CelebrityProblem.java"/>
-    <hyperlink ref="I15" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Merge_Overlapping_Interval.java"/>
-    <hyperlink ref="I12" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PostFixEvaluationConversion.java"/>
-    <hyperlink ref="I13" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PrefixEvaluationConversion.java"/>
-    <hyperlink ref="I10" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixEvaluation.java"/>
-    <hyperlink ref="I11" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixConversion.java"/>
-    <hyperlink ref="I16" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Smallest_Number_Following_Pattern.java"/>
-    <hyperlink ref="I17" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NormalStack.java"/>
-    <hyperlink ref="I18" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java"/>
-    <hyperlink ref="I19" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java"/>
-    <hyperlink ref="I20" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java"/>
-    <hyperlink ref="B49" r:id="rId37" display="https://leetcode.com/problems/valid-parentheses/"/>
+    <hyperlink ref="I7" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/StockSpan.java"/>
+    <hyperlink ref="I8" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/LargestAreaHistogram.java"/>
+    <hyperlink ref="I9" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/SlidingWindowMax.java"/>
+    <hyperlink ref="I5" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/BalancedBracket.java"/>
+    <hyperlink ref="I14" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/CelebrityProblem.java"/>
+    <hyperlink ref="I15" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Merge_Overlapping_Interval.java"/>
+    <hyperlink ref="I12" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PostFixEvaluationConversion.java"/>
+    <hyperlink ref="I13" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PrefixEvaluationConversion.java"/>
+    <hyperlink ref="I10" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixEvaluation.java"/>
+    <hyperlink ref="I11" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixConversion.java"/>
+    <hyperlink ref="I16" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Smallest_Number_Following_Pattern.java"/>
+    <hyperlink ref="I17" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NormalStack.java"/>
+    <hyperlink ref="I18" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java"/>
+    <hyperlink ref="I19" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java"/>
+    <hyperlink ref="I20" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java"/>
+    <hyperlink ref="B49" r:id="rId36" display="https://leetcode.com/problems/valid-parentheses/"/>
+    <hyperlink ref="I6" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId38"/>
@@ -6312,7 +6309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -6361,7 +6358,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>38</v>
@@ -6599,7 +6596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20:D23"/>
     </sheetView>
   </sheetViews>
@@ -6640,7 +6637,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -7071,7 +7068,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -7086,7 +7083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -7131,7 +7128,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -7331,10 +7328,10 @@
         <v>467</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7357,7 +7354,7 @@
         <v>470</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -7380,7 +7377,7 @@
         <v>468</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -7403,7 +7400,7 @@
         <v>469</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7426,7 +7423,7 @@
         <v>472</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -7449,7 +7446,7 @@
         <v>471</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -7469,13 +7466,13 @@
         <v>0</v>
       </c>
       <c r="H19" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="I19" t="s">
+        <v>501</v>
+      </c>
+      <c r="K19" s="16" t="s">
         <v>500</v>
-      </c>
-      <c r="I19" t="s">
-        <v>502</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -7495,7 +7492,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -7515,10 +7512,10 @@
         <v>0</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -7538,7 +7535,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -7558,7 +7555,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -7578,7 +7575,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -7598,7 +7595,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7618,10 +7615,10 @@
         <v>0</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -7641,17 +7638,15 @@
         <v>0</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I27" s="18" t="s">
+        <v>525</v>
+      </c>
+      <c r="J27" s="18" t="s">
         <v>526</v>
       </c>
-      <c r="J27" s="18" t="s">
-        <v>527</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>539</v>
-      </c>
+      <c r="K27" s="16"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
@@ -7679,13 +7674,13 @@
     <row r="32" spans="1:11" s="93" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A32" s="92"/>
       <c r="D32" s="94" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G32" s="95"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D34" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F34" t="s">
         <v>34</v>
@@ -7696,7 +7691,7 @@
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D35" s="16" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F35" t="s">
         <v>34</v>
@@ -7707,7 +7702,7 @@
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D36" s="16" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F36" t="s">
         <v>34</v>
@@ -7718,7 +7713,7 @@
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D37" s="16" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F37" t="s">
         <v>34</v>
@@ -7729,7 +7724,7 @@
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F38" t="s">
         <v>34</v>
@@ -7738,13 +7733,13 @@
         <v>0</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K38" s="16"/>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F39" t="s">
         <v>34</v>
@@ -7755,12 +7750,12 @@
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D40" s="16" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D41" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F41" t="s">
         <v>34</v>
@@ -7771,10 +7766,10 @@
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -7815,7 +7810,6 @@
     <hyperlink ref="K24" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java"/>
     <hyperlink ref="K25" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java"/>
     <hyperlink ref="K26" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java"/>
-    <hyperlink ref="K27" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7867,7 +7861,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 - 11:23:22.85
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="540">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1820,6 +1820,9 @@
 reverse
 manage the references
 equivalent to palindrome</t>
+  </si>
+  <si>
+    <t>CP/FoldALinkedList.java at main · spartan4cs/CP (github.com)</t>
   </si>
   <si>
     <t>CP/NGETR.java at main · spartan4cs/CP (github.com)</t>
@@ -5408,8 +5411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5555,7 +5558,7 @@
         <v>338</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -7083,7 +7086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -7646,7 +7649,9 @@
       <c r="J27" s="18" t="s">
         <v>526</v>
       </c>
-      <c r="K27" s="16"/>
+      <c r="K27" s="16" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
@@ -7810,6 +7815,7 @@
     <hyperlink ref="K24" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java"/>
     <hyperlink ref="K25" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java"/>
     <hyperlink ref="K26" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java"/>
+    <hyperlink ref="K27" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 - 13:00:33.58
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="542">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1826,6 +1826,12 @@
   </si>
   <si>
     <t>CP/NGETR.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>Loading Question... - LeetCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copy Linkedlist With Random Pointers </t>
   </si>
 </sst>
 </file>
@@ -2167,7 +2173,7 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2458,6 +2464,7 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -7084,10 +7091,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="D15" sqref="D15:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7364,7 +7371,7 @@
       <c r="A15" s="29">
         <v>11</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="104" t="s">
         <v>251</v>
       </c>
       <c r="E15" t="s">
@@ -7664,18 +7671,22 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>25</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="39" t="s">
         <v>210</v>
       </c>
       <c r="E29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:11" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="40" t="s">
+        <v>541</v>
+      </c>
+    </row>
     <row r="32" spans="1:11" s="93" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A32" s="92"/>
       <c r="D32" s="94" t="s">
@@ -7775,6 +7786,11 @@
       </c>
       <c r="D42" s="16" t="s">
         <v>505</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D43" s="16" t="s">
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -7816,6 +7832,7 @@
     <hyperlink ref="K25" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java"/>
     <hyperlink ref="K26" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java"/>
     <hyperlink ref="K27" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java"/>
+    <hyperlink ref="D43" r:id="rId38" display="https://leetcode.com/problems/intersection-of-two-linked-lists/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 - 13:55:24.28
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="548">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1828,10 +1828,34 @@
     <t>CP/NGETR.java at main · spartan4cs/CP (github.com)</t>
   </si>
   <si>
-    <t>Loading Question... - LeetCode</t>
-  </si>
-  <si>
     <t xml:space="preserve">Copy Linkedlist With Random Pointers </t>
+  </si>
+  <si>
+    <t>Copy List with Random Pointer - LeetCode</t>
+  </si>
+  <si>
+    <t>Intersection of Two Linked Lists - LeetCode</t>
+  </si>
+  <si>
+    <t>vvimp</t>
+  </si>
+  <si>
+    <t>can be done with recurion and array 
+but will take extra space
+you can do without recursion and O(n)</t>
+  </si>
+  <si>
+    <t>Reverse Linked List II - LeetCode</t>
+  </si>
+  <si>
+    <t>1. clone without random
+2.connect in zigzagorder
+3.set random pointer
+4.rearrange original list
+5.return cloned head</t>
+  </si>
+  <si>
+    <t>visualizeee all the problems</t>
   </si>
 </sst>
 </file>
@@ -2173,7 +2197,7 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2286,7 +2310,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2465,6 +2488,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -2978,7 +3003,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="95" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2986,7 +3011,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="95" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2994,7 +3019,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="95" t="s">
         <v>266</v>
       </c>
     </row>
@@ -3002,7 +3027,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="95" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3010,7 +3035,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="95" t="s">
         <v>268</v>
       </c>
     </row>
@@ -3018,7 +3043,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="D9" s="95" t="s">
         <v>269</v>
       </c>
     </row>
@@ -3026,7 +3051,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="96" t="s">
+      <c r="D10" s="95" t="s">
         <v>270</v>
       </c>
     </row>
@@ -3034,7 +3059,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="96" t="s">
+      <c r="D11" s="95" t="s">
         <v>271</v>
       </c>
     </row>
@@ -3042,7 +3067,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="96" t="s">
+      <c r="D12" s="95" t="s">
         <v>272</v>
       </c>
     </row>
@@ -3050,7 +3075,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="95" t="s">
         <v>273</v>
       </c>
     </row>
@@ -3058,7 +3083,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D14" s="82" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3066,7 +3091,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="82" t="s">
         <v>275</v>
       </c>
     </row>
@@ -3074,7 +3099,7 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="D16" s="83" t="s">
+      <c r="D16" s="82" t="s">
         <v>276</v>
       </c>
     </row>
@@ -3082,7 +3107,7 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="82" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3090,7 +3115,7 @@
       <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="82" t="s">
         <v>278</v>
       </c>
     </row>
@@ -3098,7 +3123,7 @@
       <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="D19" s="83" t="s">
+      <c r="D19" s="82" t="s">
         <v>279</v>
       </c>
     </row>
@@ -3106,7 +3131,7 @@
       <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="D20" s="83" t="s">
+      <c r="D20" s="82" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3114,7 +3139,7 @@
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="D21" s="83" t="s">
+      <c r="D21" s="82" t="s">
         <v>281</v>
       </c>
     </row>
@@ -3122,7 +3147,7 @@
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="D22" s="83" t="s">
+      <c r="D22" s="82" t="s">
         <v>282</v>
       </c>
     </row>
@@ -3130,7 +3155,7 @@
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="D23" s="83" t="s">
+      <c r="D23" s="82" t="s">
         <v>283</v>
       </c>
     </row>
@@ -3202,7 +3227,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="97" t="s">
         <v>284</v>
       </c>
     </row>
@@ -3210,7 +3235,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="97" t="s">
         <v>285</v>
       </c>
     </row>
@@ -3218,7 +3243,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="98" t="s">
+      <c r="D6" s="97" t="s">
         <v>286</v>
       </c>
     </row>
@@ -3226,7 +3251,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="98" t="s">
+      <c r="D7" s="97" t="s">
         <v>287</v>
       </c>
     </row>
@@ -3234,7 +3259,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="98" t="s">
+      <c r="D8" s="97" t="s">
         <v>288</v>
       </c>
     </row>
@@ -3242,7 +3267,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="98" t="s">
+      <c r="D9" s="97" t="s">
         <v>289</v>
       </c>
     </row>
@@ -3250,7 +3275,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="98" t="s">
+      <c r="D10" s="97" t="s">
         <v>290</v>
       </c>
     </row>
@@ -3258,7 +3283,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="98" t="s">
+      <c r="D11" s="97" t="s">
         <v>291</v>
       </c>
     </row>
@@ -3266,7 +3291,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="98" t="s">
+      <c r="D12" s="97" t="s">
         <v>292</v>
       </c>
     </row>
@@ -3274,7 +3299,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="98" t="s">
+      <c r="D13" s="97" t="s">
         <v>293</v>
       </c>
     </row>
@@ -3346,7 +3371,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="95" t="s">
         <v>294</v>
       </c>
     </row>
@@ -3354,7 +3379,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="95" t="s">
         <v>295</v>
       </c>
     </row>
@@ -3362,7 +3387,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="95" t="s">
         <v>296</v>
       </c>
     </row>
@@ -3370,7 +3395,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="95" t="s">
         <v>297</v>
       </c>
     </row>
@@ -3378,7 +3403,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="95" t="s">
         <v>298</v>
       </c>
     </row>
@@ -3386,7 +3411,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="D9" s="95" t="s">
         <v>299</v>
       </c>
     </row>
@@ -3394,7 +3419,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="96" t="s">
+      <c r="D10" s="95" t="s">
         <v>300</v>
       </c>
     </row>
@@ -3402,7 +3427,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="96" t="s">
+      <c r="D11" s="95" t="s">
         <v>301</v>
       </c>
     </row>
@@ -3410,7 +3435,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="96" t="s">
+      <c r="D12" s="95" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3418,7 +3443,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="95" t="s">
         <v>303</v>
       </c>
     </row>
@@ -3426,7 +3451,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D14" s="82" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3434,7 +3459,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="82" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3442,7 +3467,7 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="D16" s="83" t="s">
+      <c r="D16" s="82" t="s">
         <v>306</v>
       </c>
     </row>
@@ -3450,7 +3475,7 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="82" t="s">
         <v>307</v>
       </c>
     </row>
@@ -3525,7 +3550,7 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="95" t="s">
         <v>308</v>
       </c>
     </row>
@@ -3533,7 +3558,7 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="95" t="s">
         <v>310</v>
       </c>
     </row>
@@ -3541,7 +3566,7 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="95" t="s">
         <v>311</v>
       </c>
     </row>
@@ -3549,7 +3574,7 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="95" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3557,7 +3582,7 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="95" t="s">
         <v>313</v>
       </c>
     </row>
@@ -3565,7 +3590,7 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="D9" s="95" t="s">
         <v>314</v>
       </c>
     </row>
@@ -3573,7 +3598,7 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="96" t="s">
+      <c r="D10" s="95" t="s">
         <v>315</v>
       </c>
     </row>
@@ -3581,7 +3606,7 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="96" t="s">
+      <c r="D11" s="95" t="s">
         <v>316</v>
       </c>
     </row>
@@ -3589,7 +3614,7 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="96" t="s">
+      <c r="D12" s="95" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3597,7 +3622,7 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="95" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3605,7 +3630,7 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D14" s="82" t="s">
         <v>319</v>
       </c>
     </row>
@@ -3613,7 +3638,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="82" t="s">
         <v>320</v>
       </c>
     </row>
@@ -3621,7 +3646,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="83" t="s">
+      <c r="D16" s="82" t="s">
         <v>321</v>
       </c>
     </row>
@@ -3629,7 +3654,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="82" t="s">
         <v>322</v>
       </c>
     </row>
@@ -3637,7 +3662,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="82" t="s">
         <v>323</v>
       </c>
     </row>
@@ -3645,7 +3670,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="83" t="s">
+      <c r="D19" s="82" t="s">
         <v>324</v>
       </c>
     </row>
@@ -3653,7 +3678,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="83" t="s">
+      <c r="D20" s="82" t="s">
         <v>325</v>
       </c>
     </row>
@@ -3661,7 +3686,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="83" t="s">
+      <c r="D21" s="82" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3781,7 +3806,7 @@
         <v>451</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="79" t="s">
         <v>473</v>
       </c>
       <c r="E8" s="5">
@@ -3816,7 +3841,7 @@
       <c r="F9" s="25" t="s">
         <v>495</v>
       </c>
-      <c r="G9" s="91" t="s">
+      <c r="G9" s="90" t="s">
         <v>497</v>
       </c>
       <c r="H9" s="10"/>
@@ -3999,7 +4024,7 @@
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -4028,7 +4053,7 @@
       <c r="B5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="41" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -4057,7 +4082,7 @@
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="41" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -4086,7 +4111,7 @@
       <c r="B7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="41" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -4115,7 +4140,7 @@
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="41" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -4141,7 +4166,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="41" t="s">
         <v>81</v>
       </c>
       <c r="G9" s="2">
@@ -4164,7 +4189,7 @@
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="41" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -4196,7 +4221,7 @@
       <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="42" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -4228,7 +4253,7 @@
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="43" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -4257,7 +4282,7 @@
       <c r="B13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="44" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -4289,7 +4314,7 @@
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="44" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -4321,7 +4346,7 @@
       <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="44" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -4347,7 +4372,7 @@
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -4373,7 +4398,7 @@
       <c r="B17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="45" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -4402,7 +4427,7 @@
       <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="46" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -4428,7 +4453,7 @@
       <c r="B19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="48" t="s">
+      <c r="D19" s="47" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -4451,7 +4476,7 @@
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="47" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -4474,7 +4499,7 @@
       <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="47" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -4497,7 +4522,7 @@
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="48" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -4520,7 +4545,7 @@
       <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="50" t="s">
+      <c r="D23" s="49" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -4549,7 +4574,7 @@
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="51" t="s">
+      <c r="D24" s="50" t="s">
         <v>20</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -4578,7 +4603,7 @@
       <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="51" t="s">
+      <c r="D25" s="50" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -4605,7 +4630,7 @@
       <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="51" t="s">
+      <c r="D26" s="50" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -4632,7 +4657,7 @@
       <c r="B27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="51" t="s">
+      <c r="D27" s="50" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -4662,7 +4687,7 @@
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="51" t="s">
+      <c r="D28" s="50" t="s">
         <v>24</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -4689,7 +4714,7 @@
       <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="52" t="s">
+      <c r="D29" s="51" t="s">
         <v>25</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -4719,7 +4744,7 @@
       <c r="B30" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="55" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -4749,7 +4774,7 @@
       <c r="B31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="53" t="s">
+      <c r="D31" s="52" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -4779,7 +4804,7 @@
       <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="54" t="s">
+      <c r="D32" s="53" t="s">
         <v>132</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -4803,7 +4828,7 @@
       <c r="K32" s="16"/>
     </row>
     <row r="33" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="54" t="s">
+      <c r="D33" s="53" t="s">
         <v>133</v>
       </c>
       <c r="G33" s="2">
@@ -4821,7 +4846,7 @@
       <c r="B34" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="55" t="s">
+      <c r="D34" s="54" t="s">
         <v>28</v>
       </c>
       <c r="E34" s="5" t="s">
@@ -4853,7 +4878,7 @@
       <c r="K36" s="16"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D37" s="80"/>
+      <c r="D37" s="79"/>
       <c r="K37" s="16"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -4970,7 +4995,7 @@
       <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="82" t="s">
         <v>64</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -4996,7 +5021,7 @@
       <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="82" t="s">
         <v>66</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -5022,7 +5047,7 @@
       <c r="A8" s="13">
         <v>3</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="82" t="s">
         <v>65</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -5042,7 +5067,7 @@
       <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="83" t="s">
         <v>139</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -5065,7 +5090,7 @@
       <c r="A10" s="13">
         <v>5</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="83" t="s">
         <v>139</v>
       </c>
       <c r="F10" s="23" t="s">
@@ -5082,10 +5107,10 @@
       <c r="A11" s="13">
         <v>6</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="83" t="s">
         <v>168</v>
       </c>
-      <c r="F11" s="79" t="s">
+      <c r="F11" s="78" t="s">
         <v>34</v>
       </c>
       <c r="G11" s="5">
@@ -5102,7 +5127,7 @@
       <c r="A12" s="13">
         <v>7</v>
       </c>
-      <c r="D12" s="84" t="s">
+      <c r="D12" s="83" t="s">
         <v>140</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -5122,7 +5147,7 @@
       <c r="A13" s="13">
         <v>8</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="83" t="s">
         <v>144</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -5148,7 +5173,7 @@
       <c r="A14" s="13">
         <v>9</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="D14" s="81" t="s">
         <v>149</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -5174,10 +5199,10 @@
       <c r="A15" s="13">
         <v>10</v>
       </c>
-      <c r="C15" s="81" t="s">
+      <c r="C15" s="80" t="s">
         <v>479</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="D15" s="81" t="s">
         <v>151</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -5203,7 +5228,7 @@
       <c r="A16" s="13">
         <v>11</v>
       </c>
-      <c r="D16" s="82" t="s">
+      <c r="D16" s="81" t="s">
         <v>153</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -5226,7 +5251,7 @@
       <c r="A17" s="13">
         <v>12</v>
       </c>
-      <c r="D17" s="84" t="s">
+      <c r="D17" s="83" t="s">
         <v>154</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -5249,7 +5274,7 @@
       <c r="A18" s="13">
         <v>13</v>
       </c>
-      <c r="D18" s="84" t="s">
+      <c r="D18" s="83" t="s">
         <v>157</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -5272,7 +5297,7 @@
       <c r="A19" s="13">
         <v>14</v>
       </c>
-      <c r="D19" s="84" t="s">
+      <c r="D19" s="83" t="s">
         <v>159</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -5295,7 +5320,7 @@
       <c r="A20" s="13">
         <v>15</v>
       </c>
-      <c r="D20" s="84" t="s">
+      <c r="D20" s="83" t="s">
         <v>162</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -5315,7 +5340,7 @@
       <c r="A21" s="13">
         <v>16</v>
       </c>
-      <c r="D21" s="84" t="s">
+      <c r="D21" s="83" t="s">
         <v>163</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -5335,7 +5360,7 @@
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="D22" s="84" t="s">
+      <c r="D22" s="83" t="s">
         <v>166</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -5355,7 +5380,7 @@
       <c r="A23" s="13">
         <v>18</v>
       </c>
-      <c r="D23" s="85" t="s">
+      <c r="D23" s="84" t="s">
         <v>174</v>
       </c>
       <c r="I23" s="15" t="s">
@@ -5366,12 +5391,12 @@
       <c r="A24" s="13">
         <v>19</v>
       </c>
-      <c r="D24" s="85" t="s">
+      <c r="D24" s="84" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="65"/>
+      <c r="D25" s="64"/>
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
@@ -5494,7 +5519,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="56" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -5520,7 +5545,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="57" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -5546,7 +5571,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="58" t="s">
         <v>336</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -5572,7 +5597,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="50" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -5598,7 +5623,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="50" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -5621,16 +5646,16 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="69" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="71">
+      <c r="C9" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="70">
         <v>5</v>
       </c>
       <c r="G9" s="10" t="s">
@@ -5644,7 +5669,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="61" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -5673,7 +5698,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="60" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -5699,7 +5724,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="60" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -5725,16 +5750,16 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="69" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="71">
+      <c r="C13" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="70">
         <v>3</v>
       </c>
       <c r="F13" s="10" t="s">
@@ -5751,7 +5776,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="63" t="s">
         <v>48</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -5777,7 +5802,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="63" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -5800,7 +5825,7 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="63" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -5823,7 +5848,7 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="50" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -5846,7 +5871,7 @@
       <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="50" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -5866,7 +5891,7 @@
       <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="50" t="s">
         <v>54</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -5895,16 +5920,16 @@
       <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="67" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="68">
+      <c r="C20" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="67">
         <v>3</v>
       </c>
       <c r="G20" s="10" t="s">
@@ -6024,7 +6049,7 @@
       <c r="G36" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="H36" s="60"/>
+      <c r="H36" s="59"/>
       <c r="I36" s="31"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -6046,7 +6071,7 @@
       <c r="F37" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="H37" s="60"/>
+      <c r="H37" s="59"/>
       <c r="I37" s="31"/>
     </row>
     <row r="38" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6342,23 +6367,23 @@
       </c>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:9" s="73" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="103" t="s">
+    <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A2" s="102" t="s">
         <v>349</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="I2" s="74"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="75" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="28" t="s">
@@ -6367,7 +6392,7 @@
       <c r="D3" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="71" t="s">
         <v>489</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -6387,7 +6412,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="76" t="s">
         <v>413</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -6412,7 +6437,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="5"/>
@@ -6429,7 +6454,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -6452,7 +6477,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="47" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -6475,7 +6500,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="47" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -6498,7 +6523,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="47" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -6521,7 +6546,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="48" t="s">
         <v>61</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -6534,7 +6559,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="10"/>
-      <c r="G10" s="78" t="s">
+      <c r="G10" s="77" t="s">
         <v>446</v>
       </c>
       <c r="H10" s="11"/>
@@ -6556,7 +6581,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="74" t="s">
         <v>409</v>
       </c>
       <c r="G11" s="10" t="s">
@@ -6666,7 +6691,7 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="86" t="s">
+      <c r="D4" s="85" t="s">
         <v>178</v>
       </c>
       <c r="E4" t="s">
@@ -6680,7 +6705,7 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="85" t="s">
         <v>179</v>
       </c>
       <c r="E5" t="s">
@@ -6694,7 +6719,7 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="85" t="s">
         <v>180</v>
       </c>
       <c r="E6" t="s">
@@ -6708,7 +6733,7 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="85" t="s">
         <v>181</v>
       </c>
       <c r="E7" t="s">
@@ -6722,7 +6747,7 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="86" t="s">
+      <c r="D8" s="85" t="s">
         <v>182</v>
       </c>
       <c r="E8" t="s">
@@ -6736,7 +6761,7 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="85" t="s">
         <v>183</v>
       </c>
       <c r="E9" t="s">
@@ -6750,7 +6775,7 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="87" t="s">
+      <c r="D10" s="86" t="s">
         <v>184</v>
       </c>
       <c r="E10" t="s">
@@ -6764,7 +6789,7 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="87" t="s">
+      <c r="D11" s="86" t="s">
         <v>185</v>
       </c>
       <c r="E11" t="s">
@@ -6778,7 +6803,7 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="87" t="s">
+      <c r="D12" s="86" t="s">
         <v>186</v>
       </c>
       <c r="E12" t="s">
@@ -6792,7 +6817,7 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="87" t="s">
+      <c r="D13" s="86" t="s">
         <v>187</v>
       </c>
       <c r="E13" t="s">
@@ -6806,7 +6831,7 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="87" t="s">
+      <c r="D14" s="86" t="s">
         <v>188</v>
       </c>
       <c r="E14" t="s">
@@ -6820,7 +6845,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="87" t="s">
+      <c r="D15" s="86" t="s">
         <v>189</v>
       </c>
       <c r="E15" t="s">
@@ -6834,7 +6859,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="102" t="s">
+      <c r="D16" s="101" t="s">
         <v>190</v>
       </c>
       <c r="E16" t="s">
@@ -6848,7 +6873,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="102" t="s">
+      <c r="D17" s="101" t="s">
         <v>191</v>
       </c>
       <c r="E17" t="s">
@@ -6862,7 +6887,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="102" t="s">
+      <c r="D18" s="101" t="s">
         <v>192</v>
       </c>
       <c r="E18" t="s">
@@ -6876,7 +6901,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="102" t="s">
+      <c r="D19" s="101" t="s">
         <v>193</v>
       </c>
       <c r="E19" t="s">
@@ -6890,7 +6915,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="89" t="s">
+      <c r="D20" s="88" t="s">
         <v>194</v>
       </c>
       <c r="E20" t="s">
@@ -6904,7 +6929,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="89" t="s">
+      <c r="D21" s="88" t="s">
         <v>195</v>
       </c>
       <c r="E21" t="s">
@@ -6918,7 +6943,7 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="D22" s="89" t="s">
+      <c r="D22" s="88" t="s">
         <v>196</v>
       </c>
       <c r="E22" t="s">
@@ -6932,7 +6957,7 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="D23" s="89" t="s">
+      <c r="D23" s="88" t="s">
         <v>197</v>
       </c>
       <c r="E23" t="s">
@@ -6946,7 +6971,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="D24" s="90" t="s">
+      <c r="D24" s="89" t="s">
         <v>198</v>
       </c>
       <c r="E24" t="s">
@@ -6960,7 +6985,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="D25" s="90" t="s">
+      <c r="D25" s="89" t="s">
         <v>199</v>
       </c>
       <c r="E25" t="s">
@@ -6974,7 +6999,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="D26" s="90" t="s">
+      <c r="D26" s="89" t="s">
         <v>200</v>
       </c>
       <c r="E26" t="s">
@@ -6988,7 +7013,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="D27" s="90" t="s">
+      <c r="D27" s="89" t="s">
         <v>201</v>
       </c>
       <c r="E27" t="s">
@@ -7002,7 +7027,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="D28" s="88" t="s">
+      <c r="D28" s="87" t="s">
         <v>202</v>
       </c>
       <c r="E28" t="s">
@@ -7016,7 +7041,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="D29" s="88" t="s">
+      <c r="D29" s="87" t="s">
         <v>203</v>
       </c>
       <c r="E29" t="s">
@@ -7030,7 +7055,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="D30" s="88" t="s">
+      <c r="D30" s="87" t="s">
         <v>204</v>
       </c>
       <c r="E30" t="s">
@@ -7044,7 +7069,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="D31" s="88" t="s">
+      <c r="D31" s="87" t="s">
         <v>205</v>
       </c>
       <c r="E31" t="s">
@@ -7058,7 +7083,7 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="D32" s="88" t="s">
+      <c r="D32" s="87" t="s">
         <v>206</v>
       </c>
       <c r="G32" s="29">
@@ -7069,7 +7094,7 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="D33" s="88" t="s">
+      <c r="D33" s="87" t="s">
         <v>207</v>
       </c>
       <c r="G33" s="29">
@@ -7091,10 +7116,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7112,10 +7137,14 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
+      <c r="D1" s="105" t="s">
+        <v>547</v>
+      </c>
       <c r="G1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2"/>
+      <c r="D2" s="105"/>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7162,7 +7191,7 @@
       <c r="A5" s="29">
         <v>1</v>
       </c>
-      <c r="D5" s="99" t="s">
+      <c r="D5" s="98" t="s">
         <v>241</v>
       </c>
       <c r="E5" t="s">
@@ -7182,7 +7211,7 @@
       <c r="A6" s="29">
         <v>2</v>
       </c>
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="99" t="s">
         <v>242</v>
       </c>
       <c r="E6" t="s">
@@ -7202,7 +7231,7 @@
       <c r="A7" s="29">
         <v>3</v>
       </c>
-      <c r="D7" s="100" t="s">
+      <c r="D7" s="99" t="s">
         <v>243</v>
       </c>
       <c r="E7" t="s">
@@ -7222,7 +7251,7 @@
       <c r="A8" s="29">
         <v>4</v>
       </c>
-      <c r="D8" s="100" t="s">
+      <c r="D8" s="99" t="s">
         <v>244</v>
       </c>
       <c r="E8" t="s">
@@ -7242,7 +7271,7 @@
       <c r="A9" s="29">
         <v>5</v>
       </c>
-      <c r="D9" s="100" t="s">
+      <c r="D9" s="99" t="s">
         <v>245</v>
       </c>
       <c r="E9" t="s">
@@ -7262,7 +7291,7 @@
       <c r="A10" s="29">
         <v>6</v>
       </c>
-      <c r="D10" s="100" t="s">
+      <c r="D10" s="99" t="s">
         <v>246</v>
       </c>
       <c r="E10" t="s">
@@ -7282,7 +7311,7 @@
       <c r="A11" s="29">
         <v>7</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="99" t="s">
         <v>247</v>
       </c>
       <c r="E11" t="s">
@@ -7302,7 +7331,7 @@
       <c r="A12" s="29">
         <v>8</v>
       </c>
-      <c r="D12" s="100" t="s">
+      <c r="D12" s="99" t="s">
         <v>248</v>
       </c>
       <c r="E12" t="s">
@@ -7322,7 +7351,7 @@
       <c r="A13" s="29">
         <v>9</v>
       </c>
-      <c r="D13" s="100" t="s">
+      <c r="D13" s="99" t="s">
         <v>249</v>
       </c>
       <c r="E13" t="s">
@@ -7348,7 +7377,7 @@
       <c r="A14" s="29">
         <v>10</v>
       </c>
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="100" t="s">
         <v>250</v>
       </c>
       <c r="E14" t="s">
@@ -7371,7 +7400,7 @@
       <c r="A15" s="29">
         <v>11</v>
       </c>
-      <c r="D15" s="104" t="s">
+      <c r="D15" s="103" t="s">
         <v>251</v>
       </c>
       <c r="E15" t="s">
@@ -7660,7 +7689,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>24</v>
       </c>
@@ -7669,6 +7698,12 @@
       </c>
       <c r="E28" t="s">
         <v>33</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -7681,18 +7716,42 @@
       <c r="E29" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="40" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="93" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A32" s="92"/>
-      <c r="D32" s="94" t="s">
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="29">
+        <v>26</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="D30" s="104" t="s">
+        <v>540</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="1:11" s="92" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A32" s="91"/>
+      <c r="D32" s="93" t="s">
         <v>508</v>
       </c>
-      <c r="G32" s="95"/>
+      <c r="G32" s="94"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D34" s="16" t="s">
@@ -7707,18 +7766,12 @@
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D35" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="F35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" s="5">
-        <v>0</v>
+        <v>545</v>
       </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D36" s="16" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="F36" t="s">
         <v>34</v>
@@ -7729,7 +7782,7 @@
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D37" s="16" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F37" t="s">
         <v>34</v>
@@ -7740,7 +7793,7 @@
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F38" t="s">
         <v>34</v>
@@ -7748,14 +7801,10 @@
       <c r="G38" s="5">
         <v>0</v>
       </c>
-      <c r="H38" s="16" t="s">
-        <v>514</v>
-      </c>
-      <c r="K38" s="16"/>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="F39" t="s">
         <v>34</v>
@@ -7763,34 +7812,63 @@
       <c r="G39" s="5">
         <v>0</v>
       </c>
+      <c r="H39" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="K39" s="16"/>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D40" s="16" t="s">
-        <v>512</v>
+        <v>503</v>
+      </c>
+      <c r="F40" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D41" s="16" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D42" s="16" t="s">
         <v>504</v>
       </c>
-      <c r="F41" t="s">
-        <v>34</v>
-      </c>
-      <c r="G41" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C42" s="5" t="s">
+      <c r="F42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C43" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D43" s="16" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D43" s="16" t="s">
-        <v>540</v>
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D44" s="16" t="s">
+        <v>542</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D45" s="16" t="s">
+        <v>541</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7808,17 +7886,17 @@
     <hyperlink ref="K19" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Leet_mergeTwoSorterLinklist.java"/>
     <hyperlink ref="K20" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistMergeSort.java"/>
     <hyperlink ref="H21" r:id="rId13" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
-    <hyperlink ref="D42" r:id="rId14" display="https://leetcode.com/problems/remove-duplicates-from-an-unsorted-linked-list/"/>
+    <hyperlink ref="D43" r:id="rId14" display="https://leetcode.com/problems/remove-duplicates-from-an-unsorted-linked-list/"/>
     <hyperlink ref="I13" r:id="rId15" display="https://leetcode.com/problems/reverse-linked-list/"/>
-    <hyperlink ref="D39" r:id="rId16" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
-    <hyperlink ref="D35" r:id="rId17" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
+    <hyperlink ref="D40" r:id="rId16" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
+    <hyperlink ref="D36" r:id="rId17" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
     <hyperlink ref="D34" r:id="rId18" display="https://leetcode.com/problems/reverse-linked-list/"/>
-    <hyperlink ref="D37" r:id="rId19" display="https://leetcode.com/problems/linked-list-cycle/"/>
-    <hyperlink ref="D38" r:id="rId20" display="https://leetcode.com/problems/linked-list-cycle-ii/"/>
-    <hyperlink ref="D41" r:id="rId21" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/"/>
-    <hyperlink ref="D36" r:id="rId22" display="https://leetcode.com/problems/palindrome-linked-list/"/>
-    <hyperlink ref="D40" r:id="rId23" display="https://leetcode.com/problems/add-two-numbers/"/>
-    <hyperlink ref="H38" r:id="rId24" display="https://www.youtube.com/watch?v=dpqpgnTHiLs"/>
+    <hyperlink ref="D38" r:id="rId19" display="https://leetcode.com/problems/linked-list-cycle/"/>
+    <hyperlink ref="D39" r:id="rId20" display="https://leetcode.com/problems/linked-list-cycle-ii/"/>
+    <hyperlink ref="D42" r:id="rId21" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/"/>
+    <hyperlink ref="D37" r:id="rId22" display="https://leetcode.com/problems/palindrome-linked-list/"/>
+    <hyperlink ref="D41" r:id="rId23" display="https://leetcode.com/problems/add-two-numbers/"/>
+    <hyperlink ref="H39" r:id="rId24" display="https://www.youtube.com/watch?v=dpqpgnTHiLs"/>
     <hyperlink ref="K22" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/OddEvenLinklist.java"/>
     <hyperlink ref="K21" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/RemoveDuplicatesFromSortedLL.java"/>
     <hyperlink ref="K15" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java"/>
@@ -7832,9 +7910,12 @@
     <hyperlink ref="K25" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java"/>
     <hyperlink ref="K26" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java"/>
     <hyperlink ref="K27" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java"/>
-    <hyperlink ref="D43" r:id="rId38" display="https://leetcode.com/problems/intersection-of-two-linked-lists/"/>
+    <hyperlink ref="D45" r:id="rId38" display="https://leetcode.com/problems/copy-list-with-random-pointer/"/>
+    <hyperlink ref="D44" r:id="rId39" display="https://leetcode.com/problems/intersection-of-two-linked-lists/"/>
+    <hyperlink ref="D35" r:id="rId40" display="https://leetcode.com/problems/reverse-linked-list-ii/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
 
@@ -7903,7 +7984,7 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="95" t="s">
         <v>211</v>
       </c>
       <c r="F4" t="s">
@@ -7917,7 +7998,7 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="95" t="s">
         <v>212</v>
       </c>
       <c r="F5" t="s">
@@ -7931,7 +8012,7 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="95" t="s">
         <v>213</v>
       </c>
       <c r="F6" t="s">
@@ -7945,7 +8026,7 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="95" t="s">
         <v>214</v>
       </c>
       <c r="F7" t="s">
@@ -7959,7 +8040,7 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="95" t="s">
         <v>215</v>
       </c>
       <c r="F8" t="s">
@@ -7973,7 +8054,7 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="D9" s="95" t="s">
         <v>216</v>
       </c>
       <c r="F9" t="s">
@@ -8001,7 +8082,7 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="96" t="s">
+      <c r="D11" s="95" t="s">
         <v>218</v>
       </c>
       <c r="F11" t="s">
@@ -8015,7 +8096,7 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="96" t="s">
+      <c r="D12" s="95" t="s">
         <v>219</v>
       </c>
       <c r="F12" t="s">
@@ -8029,7 +8110,7 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="95" t="s">
         <v>220</v>
       </c>
       <c r="F13" t="s">
@@ -8043,7 +8124,7 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="96" t="s">
+      <c r="D14" s="95" t="s">
         <v>221</v>
       </c>
     </row>
@@ -8051,7 +8132,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="82" t="s">
         <v>222</v>
       </c>
     </row>
@@ -8059,7 +8140,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="83" t="s">
+      <c r="D16" s="82" t="s">
         <v>223</v>
       </c>
     </row>
@@ -8067,7 +8148,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="82" t="s">
         <v>224</v>
       </c>
     </row>
@@ -8075,7 +8156,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="82" t="s">
         <v>225</v>
       </c>
     </row>
@@ -8083,7 +8164,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="83" t="s">
+      <c r="D19" s="82" t="s">
         <v>226</v>
       </c>
     </row>
@@ -8091,7 +8172,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="83" t="s">
+      <c r="D20" s="82" t="s">
         <v>227</v>
       </c>
     </row>
@@ -8099,7 +8180,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="83" t="s">
+      <c r="D21" s="82" t="s">
         <v>228</v>
       </c>
     </row>
@@ -8107,7 +8188,7 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="D22" s="83" t="s">
+      <c r="D22" s="82" t="s">
         <v>229</v>
       </c>
     </row>
@@ -8115,7 +8196,7 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="D23" s="83" t="s">
+      <c r="D23" s="82" t="s">
         <v>230</v>
       </c>
     </row>
@@ -8123,7 +8204,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="D24" s="97" t="s">
+      <c r="D24" s="96" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8131,7 +8212,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="D25" s="97" t="s">
+      <c r="D25" s="96" t="s">
         <v>232</v>
       </c>
     </row>
@@ -8139,7 +8220,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="D26" s="97" t="s">
+      <c r="D26" s="96" t="s">
         <v>233</v>
       </c>
     </row>
@@ -8147,7 +8228,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="D27" s="97" t="s">
+      <c r="D27" s="96" t="s">
         <v>234</v>
       </c>
     </row>
@@ -8155,7 +8236,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="D28" s="97" t="s">
+      <c r="D28" s="96" t="s">
         <v>235</v>
       </c>
     </row>
@@ -8163,7 +8244,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="D29" s="97" t="s">
+      <c r="D29" s="96" t="s">
         <v>236</v>
       </c>
     </row>
@@ -8171,7 +8252,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="D30" s="97" t="s">
+      <c r="D30" s="96" t="s">
         <v>237</v>
       </c>
     </row>
@@ -8179,7 +8260,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="D31" s="97" t="s">
+      <c r="D31" s="96" t="s">
         <v>238</v>
       </c>
     </row>
@@ -8187,7 +8268,7 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="D32" s="97" t="s">
+      <c r="D32" s="96" t="s">
         <v>239</v>
       </c>
     </row>
@@ -8195,7 +8276,7 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="D33" s="97" t="s">
+      <c r="D33" s="96" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 - 16:23:53.27
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="551">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1856,6 +1856,18 @@
   </si>
   <si>
     <t>visualizeee all the problems</t>
+  </si>
+  <si>
+    <t>Note: when I create my own linklist what all things are required</t>
+  </si>
+  <si>
+    <t>when I create java linklist wht all things I get</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for recursion understand the references ans
+reference pass hot he at next level
+aur jab vo stack se nikalte eh tab refernce remove hota he 
+lekin data us obj pe present hota he  </t>
   </si>
 </sst>
 </file>
@@ -2197,7 +2209,7 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2490,6 +2502,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -2827,10 +2846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J18"/>
+  <dimension ref="B2:K18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2840,83 +2859,87 @@
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>119</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="107" t="s">
         <v>122</v>
       </c>
-      <c r="J2" t="s">
+      <c r="G2" s="107"/>
+      <c r="J2" s="108" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K2" s="108"/>
+    </row>
+    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>121</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
         <v>48</v>
       </c>
       <c r="J3" s="16" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>528</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>529</v>
       </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
       <c r="J4" s="16"/>
     </row>
-    <row r="5" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>527</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <v>97</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>392</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="5">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>494</v>
       </c>
@@ -2928,6 +2951,9 @@
       <c r="E18" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" display="https://www.geeksforgeeks.org/java-tricks-competitive-programming-java-8/"/>
     <hyperlink ref="J5" r:id="rId2" display="https://www.geeksforgeeks.org/fast-io-in-java-in-competitive-programming/"/>
@@ -3951,7 +3977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -4912,7 +4938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -5443,7 +5469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -6345,7 +6371,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6631,7 +6657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20:D23"/>
     </sheetView>
   </sheetViews>
@@ -7116,10 +7142,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7128,6 +7154,7 @@
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="39.7109375" customWidth="1"/>
     <col min="9" max="9" width="42.7109375" customWidth="1"/>
@@ -7142,137 +7169,82 @@
       </c>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="D2" s="105"/>
+      <c r="D2" s="106" t="s">
+        <v>548</v>
+      </c>
+      <c r="E2" s="106" t="s">
+        <v>549</v>
+      </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="D3" s="105"/>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="D4" s="105"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="D5" s="105"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="D6" s="105"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D7" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G7" s="30" t="s">
         <v>489</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I7" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J7" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K7" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K4" s="16" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="29">
-        <v>1</v>
-      </c>
-      <c r="D5" s="98" t="s">
-        <v>241</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
-        <v>2</v>
-      </c>
-      <c r="D6" s="99" t="s">
-        <v>242</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="29">
-        <v>3</v>
-      </c>
-      <c r="D7" s="99" t="s">
-        <v>243</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
-        <v>4</v>
-      </c>
-      <c r="D8" s="99" t="s">
-        <v>244</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="16" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
-        <v>5</v>
-      </c>
-      <c r="D9" s="99" t="s">
-        <v>245</v>
+        <v>1</v>
+      </c>
+      <c r="D9" s="98" t="s">
+        <v>241</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -7289,10 +7261,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D10" s="99" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -7309,10 +7281,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D11" s="99" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
@@ -7329,10 +7301,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D12" s="99" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
@@ -7347,12 +7319,12 @@
         <v>450</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D13" s="99" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -7363,22 +7335,16 @@
       <c r="G13" s="5">
         <v>1</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>467</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>506</v>
-      </c>
       <c r="K13" s="16" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
-        <v>10</v>
-      </c>
-      <c r="D14" s="100" t="s">
-        <v>250</v>
+        <v>6</v>
+      </c>
+      <c r="D14" s="99" t="s">
+        <v>246</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -7389,19 +7355,16 @@
       <c r="G14" s="5">
         <v>1</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>470</v>
-      </c>
       <c r="K14" s="16" t="s">
-        <v>522</v>
+        <v>450</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
-        <v>11</v>
-      </c>
-      <c r="D15" s="103" t="s">
-        <v>251</v>
+        <v>7</v>
+      </c>
+      <c r="D15" s="99" t="s">
+        <v>247</v>
       </c>
       <c r="E15" t="s">
         <v>33</v>
@@ -7412,19 +7375,16 @@
       <c r="G15" s="5">
         <v>1</v>
       </c>
-      <c r="H15" s="18" t="s">
-        <v>468</v>
-      </c>
       <c r="K15" s="16" t="s">
-        <v>517</v>
+        <v>450</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
-        <v>12</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>252</v>
+        <v>8</v>
+      </c>
+      <c r="D16" s="99" t="s">
+        <v>248</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
@@ -7435,19 +7395,16 @@
       <c r="G16" s="5">
         <v>1</v>
       </c>
-      <c r="H16" s="18" t="s">
-        <v>469</v>
-      </c>
       <c r="K16" s="16" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
-        <v>13</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>253</v>
+        <v>9</v>
+      </c>
+      <c r="D17" s="99" t="s">
+        <v>249</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
@@ -7459,18 +7416,21 @@
         <v>1</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>472</v>
+        <v>467</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>506</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
-        <v>14</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>254</v>
+        <v>10</v>
+      </c>
+      <c r="D18" s="100" t="s">
+        <v>250</v>
       </c>
       <c r="E18" t="s">
         <v>33</v>
@@ -7482,18 +7442,18 @@
         <v>1</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
-        <v>15</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>255</v>
+        <v>11</v>
+      </c>
+      <c r="D19" s="103" t="s">
+        <v>251</v>
       </c>
       <c r="E19" t="s">
         <v>33</v>
@@ -7502,24 +7462,21 @@
         <v>34</v>
       </c>
       <c r="G19" s="5">
-        <v>0</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="I19" t="s">
-        <v>501</v>
+        <v>1</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>468</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>500</v>
+        <v>517</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
@@ -7528,18 +7485,21 @@
         <v>34</v>
       </c>
       <c r="G20" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>469</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
@@ -7548,21 +7508,21 @@
         <v>34</v>
       </c>
       <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>503</v>
+        <v>1</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>472</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>209</v>
+        <v>254</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
@@ -7571,18 +7531,21 @@
         <v>34</v>
       </c>
       <c r="G22" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>471</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -7593,16 +7556,22 @@
       <c r="G23" s="5">
         <v>0</v>
       </c>
+      <c r="H23" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="I23" t="s">
+        <v>501</v>
+      </c>
       <c r="K23" s="16" t="s">
-        <v>523</v>
+        <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -7614,15 +7583,15 @@
         <v>0</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>534</v>
+        <v>502</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -7633,16 +7602,19 @@
       <c r="G25" s="5">
         <v>0</v>
       </c>
+      <c r="H25" s="16" t="s">
+        <v>503</v>
+      </c>
       <c r="K25" s="16" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>261</v>
+        <v>209</v>
       </c>
       <c r="E26" t="s">
         <v>33</v>
@@ -7653,19 +7625,16 @@
       <c r="G26" s="5">
         <v>0</v>
       </c>
-      <c r="H26" s="18" t="s">
-        <v>524</v>
-      </c>
       <c r="K26" s="16" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
@@ -7676,243 +7645,329 @@
       <c r="G27" s="5">
         <v>0</v>
       </c>
-      <c r="H27" s="18" t="s">
-        <v>537</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>525</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>526</v>
-      </c>
       <c r="K27" s="16" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E28" t="s">
         <v>33</v>
       </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
       <c r="G28" s="5">
         <v>0</v>
       </c>
-      <c r="H28" s="18" t="s">
-        <v>544</v>
+      <c r="K28" s="16" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
+        <v>21</v>
+      </c>
+      <c r="D29" s="39" t="s">
+        <v>260</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="29">
+        <v>22</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>524</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="29">
+        <v>23</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>262</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>537</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>525</v>
+      </c>
+      <c r="J31" s="18" t="s">
+        <v>526</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="29">
+        <v>24</v>
+      </c>
+      <c r="D32" s="39" t="s">
+        <v>263</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>544</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="29">
         <v>25</v>
       </c>
-      <c r="D29" s="39" t="s">
+      <c r="D33" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="E29" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="29">
+      <c r="E33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="29">
         <v>26</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="D30" s="104" t="s">
+      <c r="D34" s="104" t="s">
         <v>540</v>
       </c>
-      <c r="E30" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="5">
-        <v>0</v>
-      </c>
-      <c r="H30" s="18" t="s">
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0</v>
+      </c>
+      <c r="H34" s="18" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H31" s="18"/>
-    </row>
-    <row r="32" spans="1:11" s="92" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A32" s="91"/>
-      <c r="D32" s="93" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="1:11" s="92" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A36" s="91"/>
+      <c r="D36" s="93" t="s">
         <v>508</v>
       </c>
-      <c r="G32" s="94"/>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D34" s="16" t="s">
+      <c r="G36" s="94"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D38" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="F34" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D35" s="16" t="s">
+      <c r="F38" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D39" s="16" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D36" s="16" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D40" s="16" t="s">
         <v>499</v>
       </c>
-      <c r="F36" t="s">
-        <v>34</v>
-      </c>
-      <c r="G36" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D37" s="16" t="s">
+      <c r="F40" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D41" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F37" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D38" s="16" t="s">
+      <c r="F41" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D42" s="16" t="s">
         <v>509</v>
       </c>
-      <c r="F38" t="s">
-        <v>34</v>
-      </c>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D39" s="16" t="s">
+      <c r="F42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D43" s="16" t="s">
         <v>511</v>
       </c>
-      <c r="F39" t="s">
-        <v>34</v>
-      </c>
-      <c r="G39" s="5">
-        <v>0</v>
-      </c>
-      <c r="H39" s="16" t="s">
+      <c r="F43" t="s">
+        <v>34</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+      <c r="H43" s="16" t="s">
         <v>514</v>
       </c>
-      <c r="K39" s="16"/>
-    </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D40" s="16" t="s">
+      <c r="K43" s="16"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D44" s="16" t="s">
         <v>503</v>
       </c>
-      <c r="F40" t="s">
-        <v>34</v>
-      </c>
-      <c r="G40" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D41" s="16" t="s">
+      <c r="F44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D45" s="16" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D42" s="16" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D46" s="16" t="s">
         <v>504</v>
       </c>
-      <c r="F42" t="s">
-        <v>34</v>
-      </c>
-      <c r="G42" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C43" s="5" t="s">
+      <c r="F46" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C47" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D47" s="16" t="s">
         <v>505</v>
       </c>
-      <c r="G43" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D44" s="16" t="s">
+      <c r="G47" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D48" s="16" t="s">
         <v>542</v>
       </c>
-      <c r="G44" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D45" s="16" t="s">
+      <c r="G48" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D49" s="16" t="s">
         <v>541</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G49" s="5">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K4" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K5" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K6" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K7" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K8" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K9" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K10" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K11" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K12" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="H19" r:id="rId10" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
-    <hyperlink ref="K19" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Leet_mergeTwoSorterLinklist.java"/>
-    <hyperlink ref="K20" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistMergeSort.java"/>
-    <hyperlink ref="H21" r:id="rId13" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
-    <hyperlink ref="D43" r:id="rId14" display="https://leetcode.com/problems/remove-duplicates-from-an-unsorted-linked-list/"/>
-    <hyperlink ref="I13" r:id="rId15" display="https://leetcode.com/problems/reverse-linked-list/"/>
-    <hyperlink ref="D40" r:id="rId16" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
-    <hyperlink ref="D36" r:id="rId17" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
-    <hyperlink ref="D34" r:id="rId18" display="https://leetcode.com/problems/reverse-linked-list/"/>
-    <hyperlink ref="D38" r:id="rId19" display="https://leetcode.com/problems/linked-list-cycle/"/>
-    <hyperlink ref="D39" r:id="rId20" display="https://leetcode.com/problems/linked-list-cycle-ii/"/>
-    <hyperlink ref="D42" r:id="rId21" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/"/>
-    <hyperlink ref="D37" r:id="rId22" display="https://leetcode.com/problems/palindrome-linked-list/"/>
-    <hyperlink ref="D41" r:id="rId23" display="https://leetcode.com/problems/add-two-numbers/"/>
-    <hyperlink ref="H39" r:id="rId24" display="https://www.youtube.com/watch?v=dpqpgnTHiLs"/>
-    <hyperlink ref="K22" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/OddEvenLinklist.java"/>
-    <hyperlink ref="K21" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/RemoveDuplicatesFromSortedLL.java"/>
-    <hyperlink ref="K15" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java"/>
-    <hyperlink ref="K16" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistToQueueAdapter.java"/>
-    <hyperlink ref="K17" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KthNodeFromEndOfLiklist.java"/>
-    <hyperlink ref="K18" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/MidOfLinklist.java"/>
-    <hyperlink ref="K13" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Iterative.java"/>
-    <hyperlink ref="K14" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Pointer.java"/>
-    <hyperlink ref="K23" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KReverseinLL.java"/>
-    <hyperlink ref="K24" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java"/>
-    <hyperlink ref="K25" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java"/>
-    <hyperlink ref="K26" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java"/>
-    <hyperlink ref="K27" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java"/>
-    <hyperlink ref="D45" r:id="rId38" display="https://leetcode.com/problems/copy-list-with-random-pointer/"/>
-    <hyperlink ref="D44" r:id="rId39" display="https://leetcode.com/problems/intersection-of-two-linked-lists/"/>
-    <hyperlink ref="D35" r:id="rId40" display="https://leetcode.com/problems/reverse-linked-list-ii/"/>
+    <hyperlink ref="K8" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
+    <hyperlink ref="K9" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
+    <hyperlink ref="K10" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
+    <hyperlink ref="K11" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
+    <hyperlink ref="K12" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
+    <hyperlink ref="K13" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
+    <hyperlink ref="K14" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
+    <hyperlink ref="K15" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
+    <hyperlink ref="K16" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
+    <hyperlink ref="H23" r:id="rId10" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
+    <hyperlink ref="K23" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Leet_mergeTwoSorterLinklist.java"/>
+    <hyperlink ref="K24" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistMergeSort.java"/>
+    <hyperlink ref="H25" r:id="rId13" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
+    <hyperlink ref="D47" r:id="rId14" display="https://leetcode.com/problems/remove-duplicates-from-an-unsorted-linked-list/"/>
+    <hyperlink ref="I17" r:id="rId15" display="https://leetcode.com/problems/reverse-linked-list/"/>
+    <hyperlink ref="D44" r:id="rId16" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
+    <hyperlink ref="D40" r:id="rId17" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
+    <hyperlink ref="D38" r:id="rId18" display="https://leetcode.com/problems/reverse-linked-list/"/>
+    <hyperlink ref="D42" r:id="rId19" display="https://leetcode.com/problems/linked-list-cycle/"/>
+    <hyperlink ref="D43" r:id="rId20" display="https://leetcode.com/problems/linked-list-cycle-ii/"/>
+    <hyperlink ref="D46" r:id="rId21" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/"/>
+    <hyperlink ref="D41" r:id="rId22" display="https://leetcode.com/problems/palindrome-linked-list/"/>
+    <hyperlink ref="D45" r:id="rId23" display="https://leetcode.com/problems/add-two-numbers/"/>
+    <hyperlink ref="H43" r:id="rId24" display="https://www.youtube.com/watch?v=dpqpgnTHiLs"/>
+    <hyperlink ref="K26" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/OddEvenLinklist.java"/>
+    <hyperlink ref="K25" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/RemoveDuplicatesFromSortedLL.java"/>
+    <hyperlink ref="K19" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java"/>
+    <hyperlink ref="K20" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistToQueueAdapter.java"/>
+    <hyperlink ref="K21" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KthNodeFromEndOfLiklist.java"/>
+    <hyperlink ref="K22" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/MidOfLinklist.java"/>
+    <hyperlink ref="K17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Iterative.java"/>
+    <hyperlink ref="K18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Pointer.java"/>
+    <hyperlink ref="K27" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KReverseinLL.java"/>
+    <hyperlink ref="K28" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java"/>
+    <hyperlink ref="K29" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java"/>
+    <hyperlink ref="K30" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java"/>
+    <hyperlink ref="K31" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java"/>
+    <hyperlink ref="D49" r:id="rId38" display="https://leetcode.com/problems/copy-list-with-random-pointer/"/>
+    <hyperlink ref="D48" r:id="rId39" display="https://leetcode.com/problems/intersection-of-two-linked-lists/"/>
+    <hyperlink ref="D39" r:id="rId40" display="https://leetcode.com/problems/reverse-linked-list-ii/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId41"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 - 17:03:47.81
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="553">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1848,26 +1848,35 @@
     <t>Reverse Linked List II - LeetCode</t>
   </si>
   <si>
-    <t>1. clone without random
+    <t>visualizeee all the problems</t>
+  </si>
+  <si>
+    <t>Note: when I create my own linklist what all things are required</t>
+  </si>
+  <si>
+    <t>when I create java linklist wht all things I get</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for recursion understand the references ans
+reference pass hot he at next level
+aur jab vo stack se nikalte eh tab refernce remove hota he 
+lekin data us obj pe present hota he  </t>
+  </si>
+  <si>
+    <t>CP/Add2LinkedList.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>find the differece of 2 linklist
+then move 
+move bigg list tilll difference 
+then move both simultaneously</t>
+  </si>
+  <si>
+    <t>1. clone without random pointer
 2.connect in zigzagorder
 3.set random pointer
 4.rearrange original list
 5.return cloned head</t>
-  </si>
-  <si>
-    <t>visualizeee all the problems</t>
-  </si>
-  <si>
-    <t>Note: when I create my own linklist what all things are required</t>
-  </si>
-  <si>
-    <t>when I create java linklist wht all things I get</t>
-  </si>
-  <si>
-    <t xml:space="preserve">for recursion understand the references ans
-reference pass hot he at next level
-aur jab vo stack se nikalte eh tab refernce remove hota he 
-lekin data us obj pe present hota he  </t>
   </si>
 </sst>
 </file>
@@ -2848,7 +2857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J2" sqref="J2:K2"/>
     </sheetView>
   </sheetViews>
@@ -5469,7 +5478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -7144,8 +7153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7156,7 +7165,7 @@
     <col min="4" max="4" width="51.85546875" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="39.7109375" customWidth="1"/>
+    <col min="8" max="8" width="56" customWidth="1"/>
     <col min="9" max="9" width="42.7109375" customWidth="1"/>
     <col min="10" max="10" width="36.140625" customWidth="1"/>
     <col min="11" max="11" width="29.85546875" customWidth="1"/>
@@ -7165,17 +7174,17 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="D1" s="105" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G1"/>
     </row>
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="D2" s="106" t="s">
+        <v>547</v>
+      </c>
+      <c r="E2" s="106" t="s">
         <v>548</v>
-      </c>
-      <c r="E2" s="106" t="s">
-        <v>549</v>
       </c>
       <c r="G2"/>
     </row>
@@ -7751,6 +7760,9 @@
       <c r="E32" t="s">
         <v>33</v>
       </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
       <c r="G32" s="5">
         <v>0</v>
       </c>
@@ -7758,10 +7770,13 @@
         <v>544</v>
       </c>
       <c r="I32" s="18" t="s">
+        <v>549</v>
+      </c>
+      <c r="K32" s="16" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
         <v>25</v>
       </c>
@@ -7771,8 +7786,14 @@
       <c r="E33" t="s">
         <v>33</v>
       </c>
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
       <c r="G33" s="5">
         <v>0</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7795,7 +7816,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -7886,6 +7907,12 @@
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D45" s="16" t="s">
         <v>512</v>
+      </c>
+      <c r="F45" t="s">
+        <v>34</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -7968,9 +7995,10 @@
     <hyperlink ref="D49" r:id="rId38" display="https://leetcode.com/problems/copy-list-with-random-pointer/"/>
     <hyperlink ref="D48" r:id="rId39" display="https://leetcode.com/problems/intersection-of-two-linked-lists/"/>
     <hyperlink ref="D39" r:id="rId40" display="https://leetcode.com/problems/reverse-linked-list-ii/"/>
+    <hyperlink ref="K32" r:id="rId41" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Add2LinkedList.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId41"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 - 17:55:48.70
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="554">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1837,9 +1837,6 @@
     <t>Intersection of Two Linked Lists - LeetCode</t>
   </si>
   <si>
-    <t>vvimp</t>
-  </si>
-  <si>
     <t>can be done with recurion and array 
 but will take extra space
 you can do without recursion and O(n)</t>
@@ -1877,6 +1874,12 @@
 3.set random pointer
 4.rearrange original list
 5.return cloned head</t>
+  </si>
+  <si>
+    <t>vimp</t>
+  </si>
+  <si>
+    <t>CP/IntersectionPointOfLL.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -7153,8 +7156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7174,17 +7177,17 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="D1" s="105" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G1"/>
     </row>
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="D2" s="106" t="s">
+        <v>546</v>
+      </c>
+      <c r="E2" s="106" t="s">
         <v>547</v>
-      </c>
-      <c r="E2" s="106" t="s">
-        <v>548</v>
       </c>
       <c r="G2"/>
     </row>
@@ -7767,13 +7770,13 @@
         <v>0</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I32" s="18" t="s">
+        <v>548</v>
+      </c>
+      <c r="K32" s="16" t="s">
         <v>549</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7793,7 +7796,10 @@
         <v>0</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>551</v>
+        <v>550</v>
+      </c>
+      <c r="K33" s="16" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7801,7 +7807,7 @@
         <v>26</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>543</v>
+        <v>552</v>
       </c>
       <c r="D34" s="104" t="s">
         <v>540</v>
@@ -7816,7 +7822,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -7842,7 +7848,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -7941,6 +7947,9 @@
       <c r="D48" s="16" t="s">
         <v>542</v>
       </c>
+      <c r="F48" t="s">
+        <v>34</v>
+      </c>
       <c r="G48" s="5">
         <v>0</v>
       </c>
@@ -7948,6 +7957,9 @@
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D49" s="16" t="s">
         <v>541</v>
+      </c>
+      <c r="F49" t="s">
+        <v>34</v>
       </c>
       <c r="G49" s="5">
         <v>0</v>
@@ -7996,9 +8008,10 @@
     <hyperlink ref="D48" r:id="rId39" display="https://leetcode.com/problems/intersection-of-two-linked-lists/"/>
     <hyperlink ref="D39" r:id="rId40" display="https://leetcode.com/problems/reverse-linked-list-ii/"/>
     <hyperlink ref="K32" r:id="rId41" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Add2LinkedList.java"/>
+    <hyperlink ref="K33" r:id="rId42" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/IntersectionPointOfLL.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 - 18:25:03.02
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="555">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1880,6 +1880,9 @@
   </si>
   <si>
     <t>CP/IntersectionPointOfLL.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/CopyLLwithRandomnumbers.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3989,7 +3992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -4950,7 +4953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -5481,7 +5484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -7157,7 +7160,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7823,6 +7826,9 @@
       </c>
       <c r="H34" s="18" t="s">
         <v>551</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -8009,9 +8015,10 @@
     <hyperlink ref="D39" r:id="rId40" display="https://leetcode.com/problems/reverse-linked-list-ii/"/>
     <hyperlink ref="K32" r:id="rId41" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Add2LinkedList.java"/>
     <hyperlink ref="K33" r:id="rId42" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/IntersectionPointOfLL.java"/>
+    <hyperlink ref="K34" r:id="rId43" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/CopyLLwithRandomnumbers.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 - 20:12:16.67
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="556">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1883,6 +1883,9 @@
   </si>
   <si>
     <t>CP/CopyLLwithRandomnumbers.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>concept</t>
   </si>
 </sst>
 </file>
@@ -7159,8 +7162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7181,6 +7184,9 @@
       <c r="A1"/>
       <c r="D1" s="105" t="s">
         <v>545</v>
+      </c>
+      <c r="E1" s="5">
+        <v>0</v>
       </c>
       <c r="G1"/>
     </row>
@@ -8026,8 +8032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8096,6 +8102,9 @@
       <c r="G4">
         <v>0</v>
       </c>
+      <c r="H4" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
@@ -8110,6 +8119,9 @@
       <c r="G5">
         <v>0</v>
       </c>
+      <c r="H5" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
@@ -8123,6 +8135,9 @@
       </c>
       <c r="G6">
         <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 - 21:11:36.55
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="557">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1886,6 +1886,9 @@
   </si>
   <si>
     <t>concept</t>
+  </si>
+  <si>
+    <t>CP/GenericTreeDemo.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -8033,7 +8036,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8105,6 +8108,9 @@
       <c r="H4" t="s">
         <v>555</v>
       </c>
+      <c r="K4" s="16" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
@@ -8122,6 +8128,9 @@
       <c r="H5" t="s">
         <v>555</v>
       </c>
+      <c r="K5" s="16" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
@@ -8139,6 +8148,9 @@
       <c r="H6" t="s">
         <v>555</v>
       </c>
+      <c r="K6" s="16" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
@@ -8399,6 +8411,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K4" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
+    <hyperlink ref="K5" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
+    <hyperlink ref="K6" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code on timestamp:   22-05-2021 - 21:25:52.09
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="562">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1889,6 +1889,21 @@
   </si>
   <si>
     <t>CP/GenericTreeDemo.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>[root ]- (children…..)</t>
+  </si>
+  <si>
+    <t>CP/HeightOfTree.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/SizeOfGenericTree.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/MaxAndMinGenericTree.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>level-option</t>
   </si>
 </sst>
 </file>
@@ -8036,7 +8051,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="H8" sqref="H8:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8148,6 +8163,9 @@
       <c r="H6" t="s">
         <v>555</v>
       </c>
+      <c r="I6" t="s">
+        <v>557</v>
+      </c>
       <c r="K6" s="16" t="s">
         <v>556</v>
       </c>
@@ -8165,6 +8183,15 @@
       <c r="G7">
         <v>0</v>
       </c>
+      <c r="H7" t="s">
+        <v>555</v>
+      </c>
+      <c r="I7" t="s">
+        <v>561</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
@@ -8179,6 +8206,15 @@
       <c r="G8">
         <v>0</v>
       </c>
+      <c r="H8" t="s">
+        <v>555</v>
+      </c>
+      <c r="I8" t="s">
+        <v>561</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
@@ -8193,6 +8229,15 @@
       <c r="G9">
         <v>0</v>
       </c>
+      <c r="H9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I9" t="s">
+        <v>561</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
@@ -8207,6 +8252,12 @@
       <c r="G10">
         <v>0</v>
       </c>
+      <c r="H10" t="s">
+        <v>555</v>
+      </c>
+      <c r="I10" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
@@ -8221,6 +8272,12 @@
       <c r="G11">
         <v>0</v>
       </c>
+      <c r="H11" t="s">
+        <v>555</v>
+      </c>
+      <c r="I11" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
@@ -8235,6 +8292,12 @@
       <c r="G12">
         <v>0</v>
       </c>
+      <c r="H12" t="s">
+        <v>555</v>
+      </c>
+      <c r="I12" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
@@ -8249,6 +8312,12 @@
       <c r="G13">
         <v>0</v>
       </c>
+      <c r="H13" t="s">
+        <v>555</v>
+      </c>
+      <c r="I13" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
@@ -8256,6 +8325,9 @@
       </c>
       <c r="D14" s="95" t="s">
         <v>221</v>
+      </c>
+      <c r="I14" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -8415,6 +8487,9 @@
     <hyperlink ref="K4" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
     <hyperlink ref="K5" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
     <hyperlink ref="K6" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
+    <hyperlink ref="K9" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/HeightOfTree.java"/>
+    <hyperlink ref="K7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/SizeOfGenericTree.java"/>
+    <hyperlink ref="K8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxAndMinGenericTree.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 -  2:21:42.06
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -2002,7 +2002,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2092,6 +2092,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -2228,7 +2234,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2244,8 +2250,9 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2541,18 +2548,25 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="5" xfId="15" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="15" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
     <cellStyle name="20% - Accent6" xfId="9" builtinId="50"/>
     <cellStyle name="40% - Accent1" xfId="11" builtinId="31"/>
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="4" builtinId="39"/>
     <cellStyle name="40% - Accent4" xfId="12" builtinId="43"/>
+    <cellStyle name="40% - Accent5" xfId="15" builtinId="47"/>
     <cellStyle name="40% - Accent6" xfId="6" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2902,14 +2916,14 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="107" t="s">
+      <c r="F2" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="107"/>
-      <c r="J2" s="108" t="s">
+      <c r="G2" s="108"/>
+      <c r="J2" s="109" t="s">
         <v>328</v>
       </c>
-      <c r="K2" s="108"/>
+      <c r="K2" s="109"/>
     </row>
     <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -4975,7 +4989,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6694,7 +6708,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:D23"/>
+      <selection activeCell="G4" sqref="G4:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7180,8 +7194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7292,7 +7306,7 @@
         <v>34</v>
       </c>
       <c r="G9" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>450</v>
@@ -7312,7 +7326,7 @@
         <v>34</v>
       </c>
       <c r="G10" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>450</v>
@@ -7332,7 +7346,7 @@
         <v>34</v>
       </c>
       <c r="G11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>450</v>
@@ -7352,7 +7366,7 @@
         <v>34</v>
       </c>
       <c r="G12" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>450</v>
@@ -7372,7 +7386,7 @@
         <v>34</v>
       </c>
       <c r="G13" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>450</v>
@@ -7392,7 +7406,7 @@
         <v>34</v>
       </c>
       <c r="G14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>450</v>
@@ -7412,7 +7426,7 @@
         <v>34</v>
       </c>
       <c r="G15" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>450</v>
@@ -7432,7 +7446,7 @@
         <v>34</v>
       </c>
       <c r="G16" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>450</v>
@@ -7452,7 +7466,7 @@
         <v>34</v>
       </c>
       <c r="G17" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="18" t="s">
         <v>467</v>
@@ -7478,7 +7492,7 @@
         <v>34</v>
       </c>
       <c r="G18" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18" s="18" t="s">
         <v>470</v>
@@ -7501,7 +7515,7 @@
         <v>34</v>
       </c>
       <c r="G19" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19" s="18" t="s">
         <v>468</v>
@@ -7524,7 +7538,7 @@
         <v>34</v>
       </c>
       <c r="G20" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="18" t="s">
         <v>469</v>
@@ -7547,7 +7561,7 @@
         <v>34</v>
       </c>
       <c r="G21" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H21" s="18" t="s">
         <v>472</v>
@@ -7570,7 +7584,7 @@
         <v>34</v>
       </c>
       <c r="G22" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="18" t="s">
         <v>471</v>
@@ -7593,7 +7607,7 @@
         <v>34</v>
       </c>
       <c r="G23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="16" t="s">
         <v>499</v>
@@ -7619,7 +7633,7 @@
         <v>34</v>
       </c>
       <c r="G24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>502</v>
@@ -7639,7 +7653,7 @@
         <v>34</v>
       </c>
       <c r="G25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>503</v>
@@ -7708,7 +7722,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29">
         <v>21</v>
       </c>
@@ -7732,7 +7746,7 @@
       <c r="A30" s="29">
         <v>22</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D30" s="111" t="s">
         <v>261</v>
       </c>
       <c r="E30" t="s">
@@ -7755,7 +7769,7 @@
       <c r="A31" s="29">
         <v>23</v>
       </c>
-      <c r="D31" s="39" t="s">
+      <c r="D31" s="110" t="s">
         <v>262</v>
       </c>
       <c r="E31" t="s">
@@ -7784,7 +7798,7 @@
       <c r="A32" s="29">
         <v>24</v>
       </c>
-      <c r="D32" s="39" t="s">
+      <c r="D32" s="110" t="s">
         <v>263</v>
       </c>
       <c r="E32" t="s">
@@ -7794,7 +7808,7 @@
         <v>34</v>
       </c>
       <c r="G32" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H32" s="18" t="s">
         <v>543</v>
@@ -7806,11 +7820,11 @@
         <v>549</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="29">
         <v>25</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="112" t="s">
         <v>210</v>
       </c>
       <c r="E33" t="s">
@@ -7820,7 +7834,7 @@
         <v>34</v>
       </c>
       <c r="G33" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>550</v>
@@ -7846,7 +7860,7 @@
         <v>34</v>
       </c>
       <c r="G34" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H34" s="18" t="s">
         <v>551</v>
@@ -8050,8 +8064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8117,8 +8131,8 @@
       <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="G4">
-        <v>0</v>
+      <c r="G4" s="107">
+        <v>1</v>
       </c>
       <c r="H4" t="s">
         <v>555</v>
@@ -8137,8 +8151,8 @@
       <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="G5">
-        <v>0</v>
+      <c r="G5" s="107">
+        <v>1</v>
       </c>
       <c r="H5" t="s">
         <v>555</v>
@@ -8157,8 +8171,8 @@
       <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="G6">
-        <v>0</v>
+      <c r="G6" s="107">
+        <v>1</v>
       </c>
       <c r="H6" t="s">
         <v>555</v>
@@ -8180,8 +8194,8 @@
       <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="G7">
-        <v>0</v>
+      <c r="G7" s="107">
+        <v>1</v>
       </c>
       <c r="H7" t="s">
         <v>555</v>
@@ -8203,8 +8217,8 @@
       <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="G8">
-        <v>0</v>
+      <c r="G8" s="107">
+        <v>1</v>
       </c>
       <c r="H8" t="s">
         <v>555</v>
@@ -8226,8 +8240,8 @@
       <c r="F9" t="s">
         <v>34</v>
       </c>
-      <c r="G9">
-        <v>0</v>
+      <c r="G9" s="107">
+        <v>1</v>
       </c>
       <c r="H9" t="s">
         <v>555</v>
@@ -8249,7 +8263,7 @@
       <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="107">
         <v>0</v>
       </c>
       <c r="H10" t="s">
@@ -8269,7 +8283,7 @@
       <c r="F11" t="s">
         <v>34</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="107">
         <v>0</v>
       </c>
       <c r="H11" t="s">
@@ -8289,7 +8303,7 @@
       <c r="F12" t="s">
         <v>34</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="107">
         <v>0</v>
       </c>
       <c r="H12" t="s">
@@ -8309,7 +8323,7 @@
       <c r="F13" t="s">
         <v>34</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="107">
         <v>0</v>
       </c>
       <c r="H13" t="s">

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 -  2:48:21.77
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="563">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1904,6 +1904,9 @@
   </si>
   <si>
     <t>level-option</t>
+  </si>
+  <si>
+    <t>wrong code update it</t>
   </si>
 </sst>
 </file>
@@ -2252,7 +2255,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2558,6 +2561,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="5" xfId="15" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="15" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -7195,7 +7199,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7676,7 +7680,7 @@
         <v>34</v>
       </c>
       <c r="G26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>515</v>
@@ -7696,7 +7700,10 @@
         <v>34</v>
       </c>
       <c r="G27" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H27" s="113" t="s">
+        <v>562</v>
       </c>
       <c r="K27" s="16" t="s">
         <v>523</v>
@@ -7716,7 +7723,7 @@
         <v>34</v>
       </c>
       <c r="G28" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="16" t="s">
         <v>534</v>
@@ -7736,7 +7743,7 @@
         <v>34</v>
       </c>
       <c r="G29" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" s="16" t="s">
         <v>535</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 11:52:22.76
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="569">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1891,9 +1891,6 @@
     <t>CP/GenericTreeDemo.java at main · spartan4cs/CP (github.com)</t>
   </si>
   <si>
-    <t>[root ]- (children…..)</t>
-  </si>
-  <si>
     <t>CP/HeightOfTree.java at main · spartan4cs/CP (github.com)</t>
   </si>
   <si>
@@ -1907,6 +1904,34 @@
   </si>
   <si>
     <t>wrong code update it</t>
+  </si>
+  <si>
+    <t>if you used stack , then it will be used for depth traversal</t>
+  </si>
+  <si>
+    <t>This can be done using stack 
+stack- add fist element 
+RPA
+we are implementing recurstion initerative way</t>
+  </si>
+  <si>
+    <t>depth traversal using recursion(preorder)</t>
+  </si>
+  <si>
+    <t>radial tarversal or breadth traversal(preorder)</t>
+  </si>
+  <si>
+    <t>Move along the edge in tree</t>
+  </si>
+  <si>
+    <t>[root ]- (children…..)
+we are giving preference to children</t>
+  </si>
+  <si>
+    <t>queue - add first 
+RPA
+we are giving preference to siblings
+it display in single line</t>
   </si>
 </sst>
 </file>
@@ -4031,7 +4056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -4992,8 +5017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5523,7 +5548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -6712,7 +6737,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G17"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7198,8 +7223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7703,7 +7728,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="113" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="K27" s="16" t="s">
         <v>523</v>
@@ -7763,7 +7788,7 @@
         <v>34</v>
       </c>
       <c r="G30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="18" t="s">
         <v>524</v>
@@ -7786,7 +7811,7 @@
         <v>34</v>
       </c>
       <c r="G31" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="18" t="s">
         <v>537</v>
@@ -8071,8 +8096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8168,7 +8193,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>3</v>
       </c>
@@ -8181,11 +8206,14 @@
       <c r="G6" s="107">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
-        <v>555</v>
-      </c>
-      <c r="I6" t="s">
-        <v>557</v>
+      <c r="H6" s="109" t="s">
+        <v>564</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>563</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>556</v>
@@ -8208,10 +8236,10 @@
         <v>555</v>
       </c>
       <c r="I7" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -8231,10 +8259,10 @@
         <v>555</v>
       </c>
       <c r="I8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -8254,10 +8282,10 @@
         <v>555</v>
       </c>
       <c r="I9" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -8274,13 +8302,13 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>555</v>
+        <v>566</v>
       </c>
       <c r="I10" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>8</v>
       </c>
@@ -8293,11 +8321,14 @@
       <c r="G11" s="107">
         <v>0</v>
       </c>
-      <c r="H11" t="s">
-        <v>555</v>
-      </c>
-      <c r="I11" t="s">
-        <v>561</v>
+      <c r="H11" s="109" t="s">
+        <v>565</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>568</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -8317,7 +8348,7 @@
         <v>555</v>
       </c>
       <c r="I12" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -8337,7 +8368,7 @@
         <v>555</v>
       </c>
       <c r="I13" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -8348,7 +8379,7 @@
         <v>221</v>
       </c>
       <c r="I14" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 11:55:51.87
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="572">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1932,6 +1932,15 @@
 RPA
 we are giving preference to siblings
 it display in single line</t>
+  </si>
+  <si>
+    <t>CP/TraversalInGenericTree.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/LevelOrderTraversal.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/LevelOrderLinewiseTraversal.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -8097,7 +8106,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8307,6 +8316,9 @@
       <c r="I10" t="s">
         <v>560</v>
       </c>
+      <c r="K10" s="16" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
@@ -8330,6 +8342,9 @@
       <c r="J11" s="18" t="s">
         <v>562</v>
       </c>
+      <c r="K11" s="16" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
@@ -8349,6 +8364,9 @@
       </c>
       <c r="I12" t="s">
         <v>560</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -8542,6 +8560,9 @@
     <hyperlink ref="K9" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/HeightOfTree.java"/>
     <hyperlink ref="K7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/SizeOfGenericTree.java"/>
     <hyperlink ref="K8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxAndMinGenericTree.java"/>
+    <hyperlink ref="K10" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/TraversalInGenericTree.java"/>
+    <hyperlink ref="K11" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderTraversal.java"/>
+    <hyperlink ref="K12" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 12:15:40.08
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="577">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1918,12 +1918,6 @@
     <t>depth traversal using recursion(preorder)</t>
   </si>
   <si>
-    <t>radial tarversal or breadth traversal(preorder)</t>
-  </si>
-  <si>
-    <t>Move along the edge in tree</t>
-  </si>
-  <si>
     <t>[root ]- (children…..)
 we are giving preference to children</t>
   </si>
@@ -1941,6 +1935,41 @@
   </si>
   <si>
     <t>CP/LevelOrderLinewiseTraversal.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/LevelOrderLinewiseZigzag.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>Theory</t>
+  </si>
+  <si>
+    <t>Approach1- use 2 queue
+main queue
+child queue</t>
+  </si>
+  <si>
+    <t>level-wise /radial tarversal or breadth traversal(preorder)</t>
+  </si>
+  <si>
+    <t>level wise /breath wise / radial traversal</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">similar to level order but printing in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>different line</t>
+    </r>
+  </si>
+  <si>
+    <t>Move along the node and edge in tree</t>
   </si>
 </sst>
 </file>
@@ -2138,7 +2167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2270,6 +2299,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2289,7 +2333,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2596,6 +2640,16 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="15" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -8103,467 +8157,466 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="4" max="4" width="45.140625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" customWidth="1"/>
-    <col min="9" max="9" width="46.7109375" customWidth="1"/>
-    <col min="10" max="10" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" customWidth="1"/>
+    <col min="8" max="8" width="46.7109375" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="D1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>0</v>
+      <c r="C3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>489</v>
       </c>
+      <c r="G3" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="H3" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="J3" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="B4" s="109" t="s">
+        <v>571</v>
+      </c>
+      <c r="C4" s="114" t="s">
         <v>211</v>
       </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="107">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>555</v>
-      </c>
-      <c r="K4" s="16" t="s">
+      <c r="F4" s="107"/>
+      <c r="J4" s="16" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="B5" s="109" t="s">
+        <v>571</v>
+      </c>
+      <c r="C5" s="114" t="s">
         <v>212</v>
       </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="107">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>555</v>
-      </c>
-      <c r="K5" s="16" t="s">
+      <c r="F5" s="107"/>
+      <c r="J5" s="16" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="C6" s="95" t="s">
         <v>213</v>
       </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="107">
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="107">
         <v>1</v>
       </c>
-      <c r="H6" s="109" t="s">
+      <c r="G6" s="115" t="s">
         <v>564</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>567</v>
-      </c>
-      <c r="J6" s="18" t="s">
+      <c r="H6" s="10" t="s">
+        <v>565</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>563</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="J6" s="16" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="95" t="s">
+      <c r="C7" s="95" t="s">
         <v>214</v>
       </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="107">
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="107">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
-        <v>555</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="G7" t="s">
+        <v>497</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>560</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="J7" s="16" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="95" t="s">
+      <c r="C8" s="95" t="s">
         <v>215</v>
       </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="107">
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="107">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
-        <v>555</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="G8" t="s">
+        <v>497</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>560</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="J8" s="16" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="95" t="s">
+      <c r="C9" s="95" t="s">
         <v>216</v>
       </c>
-      <c r="F9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="107">
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="107">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
-        <v>555</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="G9" t="s">
+        <v>497</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>560</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="J9" s="16" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="C10" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="F10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="107">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>566</v>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="107">
+        <v>1</v>
+      </c>
+      <c r="G10" s="117" t="s">
+        <v>497</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>560</v>
       </c>
       <c r="I10" t="s">
-        <v>560</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>576</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="95" t="s">
+      <c r="C11" s="95" t="s">
         <v>218</v>
       </c>
-      <c r="F11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="107">
-        <v>0</v>
-      </c>
-      <c r="H11" s="109" t="s">
-        <v>565</v>
-      </c>
-      <c r="I11" s="18" t="s">
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="107">
+        <v>1</v>
+      </c>
+      <c r="G11" s="116" t="s">
+        <v>573</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="J11" s="16" t="s">
         <v>568</v>
       </c>
-      <c r="J11" s="18" t="s">
-        <v>562</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="C12" s="95" t="s">
         <v>219</v>
       </c>
-      <c r="F12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="107">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>555</v>
-      </c>
-      <c r="I12" t="s">
-        <v>560</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="107">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>574</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="95" t="s">
+      <c r="C13" s="95" t="s">
         <v>220</v>
       </c>
-      <c r="F13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="107">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="107">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
         <v>555</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H13" s="11" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="16" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="95" t="s">
+      <c r="B14" s="109" t="s">
+        <v>571</v>
+      </c>
+      <c r="C14" s="114" t="s">
         <v>221</v>
       </c>
-      <c r="I14" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="C15" s="82" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="82" t="s">
+      <c r="C16" s="82" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="82" t="s">
+      <c r="C17" s="82" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="82" t="s">
+      <c r="C18" s="82" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="82" t="s">
+      <c r="C19" s="82" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="82" t="s">
+      <c r="C20" s="82" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="82" t="s">
+      <c r="C21" s="82" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="D22" s="82" t="s">
+      <c r="C22" s="82" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="D23" s="82" t="s">
+      <c r="C23" s="82" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="D24" s="96" t="s">
+      <c r="C24" s="96" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="D25" s="96" t="s">
+      <c r="C25" s="96" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="D26" s="96" t="s">
+      <c r="C26" s="96" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="D27" s="96" t="s">
+      <c r="C27" s="96" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="D28" s="96" t="s">
+      <c r="C28" s="96" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="D29" s="96" t="s">
+      <c r="C29" s="96" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="D30" s="96" t="s">
+      <c r="C30" s="96" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="D31" s="96" t="s">
+      <c r="C31" s="96" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="D32" s="96" t="s">
+      <c r="C32" s="96" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="D33" s="96" t="s">
+      <c r="C33" s="96" t="s">
         <v>240</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K4" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
-    <hyperlink ref="K5" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
-    <hyperlink ref="K6" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
-    <hyperlink ref="K9" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/HeightOfTree.java"/>
-    <hyperlink ref="K7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/SizeOfGenericTree.java"/>
-    <hyperlink ref="K8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxAndMinGenericTree.java"/>
-    <hyperlink ref="K10" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/TraversalInGenericTree.java"/>
-    <hyperlink ref="K11" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderTraversal.java"/>
-    <hyperlink ref="K12" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java"/>
+    <hyperlink ref="J4" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
+    <hyperlink ref="J5" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
+    <hyperlink ref="J6" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
+    <hyperlink ref="J9" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/HeightOfTree.java"/>
+    <hyperlink ref="J7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/SizeOfGenericTree.java"/>
+    <hyperlink ref="J8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxAndMinGenericTree.java"/>
+    <hyperlink ref="J10" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/TraversalInGenericTree.java"/>
+    <hyperlink ref="J11" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderTraversal.java"/>
+    <hyperlink ref="J12" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java"/>
+    <hyperlink ref="J13" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseZigzag.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 12:30:26.48
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="577">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1943,11 +1943,6 @@
     <t>Theory</t>
   </si>
   <si>
-    <t>Approach1- use 2 queue
-main queue
-child queue</t>
-  </si>
-  <si>
     <t>level-wise /radial tarversal or breadth traversal(preorder)</t>
   </si>
   <si>
@@ -1970,6 +1965,12 @@
   </si>
   <si>
     <t>Move along the node and edge in tree</t>
+  </si>
+  <si>
+    <t>Approach1- use 2 queue
+main queue
+child queue
+Approach2- using delimiter using single queue</t>
   </si>
 </sst>
 </file>
@@ -8160,7 +8161,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8358,7 +8359,7 @@
         <v>560</v>
       </c>
       <c r="I10" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="J10" s="16" t="s">
         <v>567</v>
@@ -8378,7 +8379,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="116" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>566</v>
@@ -8390,7 +8391,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>
@@ -8404,13 +8405,13 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
+        <v>573</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>574</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>572</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>575</v>
       </c>
       <c r="J12" s="16" t="s">
         <v>569</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 13:26:28.78
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="577">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1970,7 +1970,8 @@
     <t>Approach1- use 2 queue
 main queue
 child queue
-Approach2- using delimiter using single queue</t>
+Approach2- using delimiter using single queue
+Approach 3 -using single queue --&gt; queue size  approach</t>
   </si>
 </sst>
 </file>
@@ -8161,7 +8162,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8391,7 +8392,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 13:35:23.87
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="578">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1837,6 +1837,9 @@
     <t>Intersection of Two Linked Lists - LeetCode</t>
   </si>
   <si>
+    <t>vvimp</t>
+  </si>
+  <si>
     <t>can be done with recurion and array 
 but will take extra space
 you can do without recursion and O(n)</t>
@@ -1947,6 +1950,75 @@
   </si>
   <si>
     <t>level wise /breath wise / radial traversal</t>
+  </si>
+  <si>
+    <t>Move along the node and edge in tree</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Approach1-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> use 2 queue
+main queue
+child queue
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Approach2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- using delimiter using single queue
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Approach 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-using single queue --&gt; queue size  approach(</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1960,18 +2032,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>different line</t>
+      <t>different line
+you can find height of tree using this appraoch3)</t>
     </r>
-  </si>
-  <si>
-    <t>Move along the node and edge in tree</t>
-  </si>
-  <si>
-    <t>Approach1- use 2 queue
-main queue
-child queue
-Approach2- using delimiter using single queue
-Approach 3 -using single queue --&gt; queue size  approach</t>
   </si>
 </sst>
 </file>
@@ -7309,7 +7372,7 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="D1" s="105" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E1" s="5">
         <v>0</v>
@@ -7319,10 +7382,10 @@
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="D2" s="106" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E2" s="106" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="G2"/>
     </row>
@@ -7793,7 +7856,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="113" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="K27" s="16" t="s">
         <v>523</v>
@@ -7908,13 +7971,13 @@
         <v>2</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7934,10 +7997,10 @@
         <v>2</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7945,7 +8008,7 @@
         <v>26</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D34" s="104" t="s">
         <v>540</v>
@@ -7960,10 +8023,10 @@
         <v>2</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -7989,7 +8052,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -8162,7 +8225,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8220,14 +8283,14 @@
         <v>1</v>
       </c>
       <c r="B4" s="109" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C4" s="114" t="s">
         <v>211</v>
       </c>
       <c r="F4" s="107"/>
       <c r="J4" s="16" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8235,14 +8298,14 @@
         <v>2</v>
       </c>
       <c r="B5" s="109" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C5" s="114" t="s">
         <v>212</v>
       </c>
       <c r="F5" s="107"/>
       <c r="J5" s="16" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8259,16 +8322,16 @@
         <v>1</v>
       </c>
       <c r="G6" s="115" t="s">
+        <v>565</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>564</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>565</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>563</v>
-      </c>
       <c r="J6" s="16" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8288,10 +8351,10 @@
         <v>497</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -8311,10 +8374,10 @@
         <v>497</v>
       </c>
       <c r="H8" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="J8" s="16" t="s">
         <v>560</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8334,10 +8397,10 @@
         <v>497</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8357,13 +8420,13 @@
         <v>497</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="I10" t="s">
         <v>575</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8380,22 +8443,25 @@
         <v>1</v>
       </c>
       <c r="G11" s="116" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>543</v>
+      </c>
       <c r="C12" s="95" t="s">
         <v>219</v>
       </c>
@@ -8406,16 +8472,16 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>576</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -8432,13 +8498,13 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -8446,7 +8512,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="109" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C14" s="114" t="s">
         <v>221</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 13:57:18.57
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="578">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2032,8 +2032,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>different line
-you can find height of tree using this appraoch3)</t>
+      <t>different line.
+You can find height of tree using this appraoch3)
+aur ek level pe jyada freedom and ocntrol he</t>
     </r>
   </si>
 </sst>
@@ -2398,7 +2399,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2671,9 +2672,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="14" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="8" applyAlignment="1">
@@ -2705,9 +2703,6 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="15" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2715,6 +2710,36 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="6" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -3073,14 +3098,14 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="108" t="s">
+      <c r="F2" s="107" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="108"/>
-      <c r="J2" s="109" t="s">
+      <c r="G2" s="107"/>
+      <c r="J2" s="108" t="s">
         <v>328</v>
       </c>
-      <c r="K2" s="109"/>
+      <c r="K2" s="108"/>
     </row>
     <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3460,7 +3485,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="96" t="s">
         <v>284</v>
       </c>
     </row>
@@ -3468,7 +3493,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="96" t="s">
         <v>285</v>
       </c>
     </row>
@@ -3476,7 +3501,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="96" t="s">
         <v>286</v>
       </c>
     </row>
@@ -3484,7 +3509,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="96" t="s">
         <v>287</v>
       </c>
     </row>
@@ -3492,7 +3517,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="96" t="s">
         <v>288</v>
       </c>
     </row>
@@ -3500,7 +3525,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="96" t="s">
         <v>289</v>
       </c>
     </row>
@@ -3508,7 +3533,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="97" t="s">
+      <c r="D10" s="96" t="s">
         <v>290</v>
       </c>
     </row>
@@ -3516,7 +3541,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="97" t="s">
+      <c r="D11" s="96" t="s">
         <v>291</v>
       </c>
     </row>
@@ -3524,7 +3549,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="97" t="s">
+      <c r="D12" s="96" t="s">
         <v>292</v>
       </c>
     </row>
@@ -3532,7 +3557,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="97" t="s">
+      <c r="D13" s="96" t="s">
         <v>293</v>
       </c>
     </row>
@@ -6601,15 +6626,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="101" t="s">
         <v>349</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7092,7 +7117,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="101" t="s">
+      <c r="D16" s="100" t="s">
         <v>190</v>
       </c>
       <c r="E16" t="s">
@@ -7106,7 +7131,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="101" t="s">
+      <c r="D17" s="100" t="s">
         <v>191</v>
       </c>
       <c r="E17" t="s">
@@ -7120,7 +7145,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="101" t="s">
+      <c r="D18" s="100" t="s">
         <v>192</v>
       </c>
       <c r="E18" t="s">
@@ -7134,7 +7159,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="101" t="s">
+      <c r="D19" s="100" t="s">
         <v>193</v>
       </c>
       <c r="E19" t="s">
@@ -7371,7 +7396,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="D1" s="105" t="s">
+      <c r="D1" s="104" t="s">
         <v>546</v>
       </c>
       <c r="E1" s="5">
@@ -7381,32 +7406,32 @@
     </row>
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="D2" s="106" t="s">
+      <c r="D2" s="105" t="s">
         <v>547</v>
       </c>
-      <c r="E2" s="106" t="s">
+      <c r="E2" s="105" t="s">
         <v>548</v>
       </c>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3"/>
-      <c r="D3" s="105"/>
+      <c r="D3" s="104"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4"/>
-      <c r="D4" s="105"/>
+      <c r="D4" s="104"/>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>
-      <c r="D5" s="105"/>
+      <c r="D5" s="104"/>
       <c r="G5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6"/>
-      <c r="D6" s="105"/>
+      <c r="D6" s="104"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7453,7 +7478,7 @@
       <c r="A9" s="29">
         <v>1</v>
       </c>
-      <c r="D9" s="98" t="s">
+      <c r="D9" s="97" t="s">
         <v>241</v>
       </c>
       <c r="E9" t="s">
@@ -7473,7 +7498,7 @@
       <c r="A10" s="29">
         <v>2</v>
       </c>
-      <c r="D10" s="99" t="s">
+      <c r="D10" s="98" t="s">
         <v>242</v>
       </c>
       <c r="E10" t="s">
@@ -7493,7 +7518,7 @@
       <c r="A11" s="29">
         <v>3</v>
       </c>
-      <c r="D11" s="99" t="s">
+      <c r="D11" s="98" t="s">
         <v>243</v>
       </c>
       <c r="E11" t="s">
@@ -7513,7 +7538,7 @@
       <c r="A12" s="29">
         <v>4</v>
       </c>
-      <c r="D12" s="99" t="s">
+      <c r="D12" s="98" t="s">
         <v>244</v>
       </c>
       <c r="E12" t="s">
@@ -7533,7 +7558,7 @@
       <c r="A13" s="29">
         <v>5</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="98" t="s">
         <v>245</v>
       </c>
       <c r="E13" t="s">
@@ -7553,7 +7578,7 @@
       <c r="A14" s="29">
         <v>6</v>
       </c>
-      <c r="D14" s="99" t="s">
+      <c r="D14" s="98" t="s">
         <v>246</v>
       </c>
       <c r="E14" t="s">
@@ -7573,7 +7598,7 @@
       <c r="A15" s="29">
         <v>7</v>
       </c>
-      <c r="D15" s="99" t="s">
+      <c r="D15" s="98" t="s">
         <v>247</v>
       </c>
       <c r="E15" t="s">
@@ -7593,7 +7618,7 @@
       <c r="A16" s="29">
         <v>8</v>
       </c>
-      <c r="D16" s="99" t="s">
+      <c r="D16" s="98" t="s">
         <v>248</v>
       </c>
       <c r="E16" t="s">
@@ -7613,7 +7638,7 @@
       <c r="A17" s="29">
         <v>9</v>
       </c>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="98" t="s">
         <v>249</v>
       </c>
       <c r="E17" t="s">
@@ -7639,7 +7664,7 @@
       <c r="A18" s="29">
         <v>10</v>
       </c>
-      <c r="D18" s="100" t="s">
+      <c r="D18" s="99" t="s">
         <v>250</v>
       </c>
       <c r="E18" t="s">
@@ -7662,7 +7687,7 @@
       <c r="A19" s="29">
         <v>11</v>
       </c>
-      <c r="D19" s="103" t="s">
+      <c r="D19" s="102" t="s">
         <v>251</v>
       </c>
       <c r="E19" t="s">
@@ -7855,7 +7880,7 @@
       <c r="G27" s="5">
         <v>1</v>
       </c>
-      <c r="H27" s="113" t="s">
+      <c r="H27" s="112" t="s">
         <v>562</v>
       </c>
       <c r="K27" s="16" t="s">
@@ -7906,7 +7931,7 @@
       <c r="A30" s="29">
         <v>22</v>
       </c>
-      <c r="D30" s="111" t="s">
+      <c r="D30" s="110" t="s">
         <v>261</v>
       </c>
       <c r="E30" t="s">
@@ -7929,7 +7954,7 @@
       <c r="A31" s="29">
         <v>23</v>
       </c>
-      <c r="D31" s="110" t="s">
+      <c r="D31" s="109" t="s">
         <v>262</v>
       </c>
       <c r="E31" t="s">
@@ -7958,7 +7983,7 @@
       <c r="A32" s="29">
         <v>24</v>
       </c>
-      <c r="D32" s="110" t="s">
+      <c r="D32" s="109" t="s">
         <v>263</v>
       </c>
       <c r="E32" t="s">
@@ -7984,7 +8009,7 @@
       <c r="A33" s="29">
         <v>25</v>
       </c>
-      <c r="D33" s="112" t="s">
+      <c r="D33" s="111" t="s">
         <v>210</v>
       </c>
       <c r="E33" t="s">
@@ -8010,7 +8035,7 @@
       <c r="C34" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="D34" s="104" t="s">
+      <c r="D34" s="103" t="s">
         <v>540</v>
       </c>
       <c r="E34" t="s">
@@ -8224,8 +8249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8246,7 +8271,7 @@
       <c r="A2"/>
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
@@ -8282,13 +8307,13 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="108" t="s">
         <v>572</v>
       </c>
-      <c r="C4" s="114" t="s">
+      <c r="C4" s="116" t="s">
         <v>211</v>
       </c>
-      <c r="F4" s="107"/>
+      <c r="F4" s="106"/>
       <c r="J4" s="16" t="s">
         <v>557</v>
       </c>
@@ -8297,13 +8322,13 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="B5" s="109" t="s">
+      <c r="B5" s="108" t="s">
         <v>572</v>
       </c>
-      <c r="C5" s="114" t="s">
+      <c r="C5" s="117" t="s">
         <v>212</v>
       </c>
-      <c r="F5" s="107"/>
+      <c r="F5" s="106"/>
       <c r="J5" s="16" t="s">
         <v>557</v>
       </c>
@@ -8312,16 +8337,16 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="118" t="s">
         <v>213</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="107">
+      <c r="F6" s="106">
         <v>1</v>
       </c>
-      <c r="G6" s="115" t="s">
+      <c r="G6" s="113" t="s">
         <v>565</v>
       </c>
       <c r="H6" s="10" t="s">
@@ -8338,13 +8363,13 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="C7" s="95" t="s">
+      <c r="C7" s="118" t="s">
         <v>214</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="107">
+      <c r="F7" s="106">
         <v>1</v>
       </c>
       <c r="G7" t="s">
@@ -8361,13 +8386,13 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="C8" s="95" t="s">
+      <c r="C8" s="118" t="s">
         <v>215</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="107">
+      <c r="F8" s="106">
         <v>1</v>
       </c>
       <c r="G8" t="s">
@@ -8384,13 +8409,13 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="118" t="s">
         <v>216</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="107">
+      <c r="F9" s="106">
         <v>1</v>
       </c>
       <c r="G9" t="s">
@@ -8407,16 +8432,16 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="98" t="s">
         <v>217</v>
       </c>
       <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="107">
+      <c r="F10" s="106">
         <v>1</v>
       </c>
-      <c r="G10" s="117" t="s">
+      <c r="G10" s="115" t="s">
         <v>497</v>
       </c>
       <c r="H10" s="11" t="s">
@@ -8433,16 +8458,16 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="118" t="s">
         <v>218</v>
       </c>
       <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="107">
+      <c r="F11" s="106">
         <v>1</v>
       </c>
-      <c r="G11" s="116" t="s">
+      <c r="G11" s="114" t="s">
         <v>573</v>
       </c>
       <c r="H11" s="10" t="s">
@@ -8462,13 +8487,13 @@
       <c r="B12" t="s">
         <v>543</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="118" t="s">
         <v>219</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="107">
+      <c r="F12" s="106">
         <v>0</v>
       </c>
       <c r="G12" t="s">
@@ -8488,13 +8513,13 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="118" t="s">
         <v>220</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="107">
+      <c r="F13" s="106">
         <v>0</v>
       </c>
       <c r="G13" t="s">
@@ -8507,14 +8532,14 @@
         <v>571</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="B14" s="109" t="s">
+      <c r="B14" s="108" t="s">
         <v>572</v>
       </c>
-      <c r="C14" s="114" t="s">
+      <c r="C14" s="119" t="s">
         <v>221</v>
       </c>
       <c r="G14" s="18"/>
@@ -8523,7 +8548,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="C15" s="82" t="s">
+      <c r="C15" s="120" t="s">
         <v>222</v>
       </c>
     </row>
@@ -8531,7 +8556,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="C16" s="82" t="s">
+      <c r="C16" s="121" t="s">
         <v>223</v>
       </c>
     </row>
@@ -8539,7 +8564,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="C17" s="82" t="s">
+      <c r="C17" s="121" t="s">
         <v>224</v>
       </c>
     </row>
@@ -8547,7 +8572,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="C18" s="82" t="s">
+      <c r="C18" s="121" t="s">
         <v>225</v>
       </c>
     </row>
@@ -8555,7 +8580,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="121" t="s">
         <v>226</v>
       </c>
     </row>
@@ -8563,7 +8588,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="C20" s="82" t="s">
+      <c r="C20" s="121" t="s">
         <v>227</v>
       </c>
     </row>
@@ -8571,7 +8596,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="C21" s="82" t="s">
+      <c r="C21" s="121" t="s">
         <v>228</v>
       </c>
     </row>
@@ -8579,15 +8604,15 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="C22" s="82" t="s">
+      <c r="C22" s="121" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="122" t="s">
         <v>230</v>
       </c>
     </row>
@@ -8595,7 +8620,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="C24" s="96" t="s">
+      <c r="C24" s="123" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8603,7 +8628,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="C25" s="96" t="s">
+      <c r="C25" s="124" t="s">
         <v>232</v>
       </c>
     </row>
@@ -8611,7 +8636,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="C26" s="96" t="s">
+      <c r="C26" s="124" t="s">
         <v>233</v>
       </c>
     </row>
@@ -8619,7 +8644,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="C27" s="96" t="s">
+      <c r="C27" s="124" t="s">
         <v>234</v>
       </c>
     </row>
@@ -8627,7 +8652,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="C28" s="96" t="s">
+      <c r="C28" s="124" t="s">
         <v>235</v>
       </c>
     </row>
@@ -8635,7 +8660,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="C29" s="96" t="s">
+      <c r="C29" s="124" t="s">
         <v>236</v>
       </c>
     </row>
@@ -8643,7 +8668,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="C30" s="96" t="s">
+      <c r="C30" s="124" t="s">
         <v>237</v>
       </c>
     </row>
@@ -8651,7 +8676,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="C31" s="96" t="s">
+      <c r="C31" s="124" t="s">
         <v>238</v>
       </c>
     </row>
@@ -8659,15 +8684,15 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="C32" s="96" t="s">
+      <c r="C32" s="124" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="C33" s="96" t="s">
+      <c r="C33" s="125" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>